<commit_message>
Adding force increment algorithm v15
</commit_message>
<xml_diff>
--- a/Examples/Problems solutions.xlsx
+++ b/Examples/Problems solutions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!MyFiles\PhD\FrictionalContactFEM\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F698C33-1045-48BC-BEC7-BB71734C6D24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27390F23-1457-451F-A942-39612CF1EE8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -170,10 +170,10 @@
     <t>ЛУЧ, P не выбить из базиса</t>
   </si>
   <si>
-    <t>ЭТАП 1</t>
+    <t>ЛУЧ</t>
   </si>
   <si>
-    <t>ЛУЧ</t>
+    <t>как получить что p должно быть равно нулю здесь</t>
   </si>
 </sst>
 </file>
@@ -24948,11 +24948,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACA946C9-CC82-403B-9946-DA1124127D9B}">
-  <dimension ref="A1:AB198"/>
+  <dimension ref="A1:Y198"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z22" sqref="Z22"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25155,7 +25155,7 @@
       <c r="T3" s="2">
         <v>-1</v>
       </c>
-      <c r="U3" s="8">
+      <c r="U3" s="3">
         <v>-9.3749999999999931E-2</v>
       </c>
       <c r="V3" s="2">
@@ -25172,70 +25172,70 @@
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="8">
-        <v>0</v>
-      </c>
-      <c r="C4" s="8">
-        <v>1</v>
-      </c>
-      <c r="D4" s="8">
-        <v>0</v>
-      </c>
-      <c r="E4" s="8">
-        <v>0</v>
-      </c>
-      <c r="F4" s="8">
-        <v>0</v>
-      </c>
-      <c r="G4" s="8">
-        <v>0</v>
-      </c>
-      <c r="H4" s="8">
-        <v>0</v>
-      </c>
-      <c r="I4" s="8">
-        <v>0</v>
-      </c>
-      <c r="J4" s="8">
-        <v>0</v>
-      </c>
-      <c r="K4" s="8">
+      <c r="B4" s="3">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3">
+        <v>0</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0</v>
+      </c>
+      <c r="K4" s="3">
         <v>0.18750000000000019</v>
       </c>
-      <c r="L4" s="8">
+      <c r="L4" s="3">
         <v>-0.375</v>
       </c>
-      <c r="M4" s="8">
+      <c r="M4" s="3">
         <v>0.18750000000000039</v>
       </c>
-      <c r="N4" s="8">
-        <v>0</v>
-      </c>
-      <c r="O4" s="8">
-        <v>0</v>
-      </c>
-      <c r="P4" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="8">
-        <v>0</v>
-      </c>
-      <c r="R4" s="8">
-        <v>0</v>
-      </c>
-      <c r="S4" s="8">
-        <v>0</v>
-      </c>
-      <c r="T4" s="8">
+      <c r="N4" s="3">
+        <v>0</v>
+      </c>
+      <c r="O4" s="3">
+        <v>0</v>
+      </c>
+      <c r="P4" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>0</v>
+      </c>
+      <c r="R4" s="3">
+        <v>0</v>
+      </c>
+      <c r="S4" s="3">
+        <v>0</v>
+      </c>
+      <c r="T4" s="3">
         <v>-1</v>
       </c>
-      <c r="U4" s="8">
+      <c r="U4" s="3">
         <v>0.68749999999999989</v>
       </c>
-      <c r="V4" s="8">
+      <c r="V4" s="3">
         <v>-0.68749999999999989</v>
       </c>
-      <c r="W4" s="8">
+      <c r="W4" s="3">
         <v>1</v>
       </c>
       <c r="X4">
@@ -25306,7 +25306,7 @@
       <c r="T5" s="2">
         <v>-1</v>
       </c>
-      <c r="U5" s="8">
+      <c r="U5" s="3">
         <v>0.40625000000000011</v>
       </c>
       <c r="V5" s="2">
@@ -25380,7 +25380,7 @@
       <c r="T6" s="2">
         <v>-1</v>
       </c>
-      <c r="U6" s="8">
+      <c r="U6" s="3">
         <v>-1.8749999999999989E-2</v>
       </c>
       <c r="V6" s="2">
@@ -25451,7 +25451,7 @@
       <c r="T7" s="2">
         <v>-1</v>
       </c>
-      <c r="U7" s="8">
+      <c r="U7" s="3">
         <v>0.13750000000000001</v>
       </c>
       <c r="V7" s="2">
@@ -25525,7 +25525,7 @@
       <c r="T8" s="2">
         <v>-1</v>
       </c>
-      <c r="U8" s="8">
+      <c r="U8" s="3">
         <v>8.1250000000000017E-2</v>
       </c>
       <c r="V8" s="2">
@@ -25599,7 +25599,7 @@
       <c r="T9" s="2">
         <v>-1</v>
       </c>
-      <c r="U9" s="8">
+      <c r="U9" s="3">
         <v>-1.8749999999999989E-2</v>
       </c>
       <c r="V9" s="2">
@@ -25670,7 +25670,7 @@
       <c r="T10" s="2">
         <v>-1</v>
       </c>
-      <c r="U10" s="8">
+      <c r="U10" s="3">
         <v>0.13750000000000001</v>
       </c>
       <c r="V10" s="2">
@@ -25744,7 +25744,7 @@
       <c r="T11" s="2">
         <v>-1</v>
       </c>
-      <c r="U11" s="8">
+      <c r="U11" s="3">
         <v>8.1250000000000017E-2</v>
       </c>
       <c r="V11" s="2">
@@ -25853,7 +25853,7 @@
       <c r="K14" s="2">
         <v>-6.8181818181818288E-2</v>
       </c>
-      <c r="L14" s="8">
+      <c r="L14" s="3">
         <v>0.1363636363636371</v>
       </c>
       <c r="M14" s="2">
@@ -25930,7 +25930,7 @@
       <c r="K15" s="2">
         <v>0.27272727272727298</v>
       </c>
-      <c r="L15" s="8">
+      <c r="L15" s="3">
         <v>-0.54545454545454553</v>
       </c>
       <c r="M15" s="2">
@@ -25974,77 +25974,77 @@
       <c r="A16">
         <v>2</v>
       </c>
-      <c r="B16" s="8">
-        <v>0</v>
-      </c>
-      <c r="C16" s="8">
+      <c r="B16" s="3">
+        <v>0</v>
+      </c>
+      <c r="C16" s="3">
         <v>-0.59090909090909105</v>
       </c>
-      <c r="D16" s="8">
-        <v>1</v>
-      </c>
-      <c r="E16" s="8">
-        <v>0</v>
-      </c>
-      <c r="F16" s="8">
-        <v>0</v>
-      </c>
-      <c r="G16" s="8">
-        <v>0</v>
-      </c>
-      <c r="H16" s="8">
-        <v>0</v>
-      </c>
-      <c r="I16" s="8">
-        <v>0</v>
-      </c>
-      <c r="J16" s="8">
-        <v>0</v>
-      </c>
-      <c r="K16" s="8">
+      <c r="D16" s="3">
+        <v>1</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0</v>
+      </c>
+      <c r="H16" s="3">
+        <v>0</v>
+      </c>
+      <c r="I16" s="3">
+        <v>0</v>
+      </c>
+      <c r="J16" s="3">
+        <v>0</v>
+      </c>
+      <c r="K16" s="3">
         <v>-0.2045454545454547</v>
       </c>
-      <c r="L16" s="8">
+      <c r="L16" s="3">
         <v>0.40909090909090928</v>
       </c>
-      <c r="M16" s="8">
+      <c r="M16" s="3">
         <v>-0.20454545454545481</v>
       </c>
-      <c r="N16" s="8">
-        <v>0</v>
-      </c>
-      <c r="O16" s="8">
-        <v>0</v>
-      </c>
-      <c r="P16" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="8">
-        <v>0</v>
-      </c>
-      <c r="R16" s="8">
-        <v>0</v>
-      </c>
-      <c r="S16" s="8">
-        <v>0</v>
-      </c>
-      <c r="T16" s="8">
+      <c r="N16" s="3">
+        <v>0</v>
+      </c>
+      <c r="O16" s="3">
+        <v>0</v>
+      </c>
+      <c r="P16" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>0</v>
+      </c>
+      <c r="R16" s="3">
+        <v>0</v>
+      </c>
+      <c r="S16" s="3">
+        <v>0</v>
+      </c>
+      <c r="T16" s="3">
         <v>-0.40909090909090889</v>
       </c>
-      <c r="U16" s="8">
-        <v>0</v>
-      </c>
-      <c r="V16" s="8">
-        <v>0</v>
-      </c>
-      <c r="W16" s="8">
+      <c r="U16" s="3">
+        <v>0</v>
+      </c>
+      <c r="V16" s="3">
+        <v>0</v>
+      </c>
+      <c r="W16" s="3">
         <v>0.40909090909090889</v>
       </c>
       <c r="X16">
         <v>0.99999999999999922</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>3</v>
       </c>
@@ -26078,7 +26078,7 @@
       <c r="K17" s="2">
         <v>-1.363636363636366E-2</v>
       </c>
-      <c r="L17" s="8">
+      <c r="L17" s="3">
         <v>2.7272727272727421E-2</v>
       </c>
       <c r="M17" s="2">
@@ -26118,7 +26118,7 @@
         <v>37.666666666666458</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>4</v>
       </c>
@@ -26152,7 +26152,7 @@
       <c r="K18" s="2">
         <v>0</v>
       </c>
-      <c r="L18" s="8">
+      <c r="L18" s="3">
         <v>0</v>
       </c>
       <c r="M18" s="2">
@@ -26189,7 +26189,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>5</v>
       </c>
@@ -26223,7 +26223,7 @@
       <c r="K19" s="2">
         <v>-4.090909090909095E-2</v>
       </c>
-      <c r="L19" s="8">
+      <c r="L19" s="3">
         <v>8.1818181818181845E-2</v>
       </c>
       <c r="M19" s="2">
@@ -26263,7 +26263,7 @@
         <v>10.77777777777778</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>6</v>
       </c>
@@ -26297,7 +26297,7 @@
       <c r="K20" s="2">
         <v>-1.363636363636366E-2</v>
       </c>
-      <c r="L20" s="8">
+      <c r="L20" s="3">
         <v>2.7272727272727421E-2</v>
       </c>
       <c r="M20" s="2">
@@ -26337,7 +26337,7 @@
         <v>37.666666666666458</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>7</v>
       </c>
@@ -26371,7 +26371,7 @@
       <c r="K21" s="2">
         <v>0</v>
       </c>
-      <c r="L21" s="8">
+      <c r="L21" s="3">
         <v>0</v>
       </c>
       <c r="M21" s="2">
@@ -26408,7 +26408,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>8</v>
       </c>
@@ -26442,7 +26442,7 @@
       <c r="K22" s="2">
         <v>-4.090909090909095E-2</v>
       </c>
-      <c r="L22" s="8">
+      <c r="L22" s="3">
         <v>8.1818181818181845E-2</v>
       </c>
       <c r="M22" s="2">
@@ -26482,7 +26482,7 @@
         <v>10.77777777777778</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>0</v>
       </c>
@@ -26543,8 +26543,14 @@
       <c r="U24">
         <v>19</v>
       </c>
-    </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="X24" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>0</v>
       </c>
@@ -26581,7 +26587,7 @@
       <c r="L25" s="2">
         <v>0</v>
       </c>
-      <c r="M25" s="8">
+      <c r="M25" s="3">
         <v>-1.9428902930940239E-16</v>
       </c>
       <c r="N25" s="2">
@@ -26618,88 +26624,81 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>19</v>
       </c>
-      <c r="B26" s="8">
-        <v>0</v>
-      </c>
-      <c r="C26" s="8">
+      <c r="B26" s="2">
+        <v>0</v>
+      </c>
+      <c r="C26" s="2">
         <v>0.66666666666666707</v>
       </c>
-      <c r="D26" s="8">
+      <c r="D26" s="2">
         <v>1.333333333333333</v>
       </c>
-      <c r="E26" s="8">
-        <v>0</v>
-      </c>
-      <c r="F26" s="8">
-        <v>0</v>
-      </c>
-      <c r="G26" s="8">
-        <v>0</v>
-      </c>
-      <c r="H26" s="8">
-        <v>0</v>
-      </c>
-      <c r="I26" s="8">
-        <v>0</v>
-      </c>
-      <c r="J26" s="8">
-        <v>0</v>
-      </c>
-      <c r="K26" s="8">
+      <c r="E26" s="2">
+        <v>0</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0</v>
+      </c>
+      <c r="G26" s="2">
+        <v>0</v>
+      </c>
+      <c r="H26" s="2">
+        <v>0</v>
+      </c>
+      <c r="I26" s="2">
+        <v>0</v>
+      </c>
+      <c r="J26" s="2">
+        <v>0</v>
+      </c>
+      <c r="K26" s="2">
         <v>2.2204460492503131E-16</v>
       </c>
-      <c r="L26" s="8">
-        <v>0</v>
-      </c>
-      <c r="M26" s="8">
+      <c r="L26" s="2">
+        <v>0</v>
+      </c>
+      <c r="M26" s="3">
         <v>3.3306690738754701E-16</v>
       </c>
-      <c r="N26" s="8">
-        <v>0</v>
-      </c>
-      <c r="O26" s="8">
-        <v>0</v>
-      </c>
-      <c r="P26" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q26" s="8">
-        <v>0</v>
-      </c>
-      <c r="R26" s="8">
-        <v>0</v>
-      </c>
-      <c r="S26" s="8">
-        <v>0</v>
-      </c>
-      <c r="T26" s="8">
+      <c r="N26" s="2">
+        <v>0</v>
+      </c>
+      <c r="O26" s="2">
+        <v>0</v>
+      </c>
+      <c r="P26" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="2">
+        <v>0</v>
+      </c>
+      <c r="R26" s="2">
+        <v>0</v>
+      </c>
+      <c r="S26" s="2">
+        <v>0</v>
+      </c>
+      <c r="T26" s="2">
         <v>-2</v>
       </c>
-      <c r="U26" s="8">
-        <v>1</v>
-      </c>
-      <c r="V26" s="8">
+      <c r="U26" s="2">
+        <v>1</v>
+      </c>
+      <c r="V26" s="2">
         <v>-1</v>
       </c>
-      <c r="W26" s="8">
+      <c r="W26" s="2">
         <v>2</v>
-      </c>
-      <c r="X26">
-        <v>6004799503160661</v>
       </c>
       <c r="Y26">
         <v>11</v>
       </c>
-      <c r="AB26">
-        <f>M15-L15*M27</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>10</v>
       </c>
@@ -26736,7 +26735,7 @@
       <c r="L27" s="2">
         <v>1</v>
       </c>
-      <c r="M27" s="8">
+      <c r="M27" s="3">
         <v>-0.50000000000000044</v>
       </c>
       <c r="N27" s="2">
@@ -26770,7 +26769,7 @@
         <v>0.99999999999999922</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>3</v>
       </c>
@@ -26807,7 +26806,7 @@
       <c r="L28" s="2">
         <v>0</v>
       </c>
-      <c r="M28" s="8">
+      <c r="M28" s="3">
         <v>-3.8163916471489762E-17</v>
       </c>
       <c r="N28" s="2">
@@ -26841,7 +26840,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>4</v>
       </c>
@@ -26878,7 +26877,7 @@
       <c r="L29" s="2">
         <v>0</v>
       </c>
-      <c r="M29" s="8">
+      <c r="M29" s="3">
         <v>0</v>
       </c>
       <c r="N29" s="2">
@@ -26912,7 +26911,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>5</v>
       </c>
@@ -26949,7 +26948,7 @@
       <c r="L30" s="2">
         <v>-1.387778780781446E-17</v>
       </c>
-      <c r="M30" s="8">
+      <c r="M30" s="3">
         <v>-1.387778780781446E-17</v>
       </c>
       <c r="N30" s="2">
@@ -26983,7 +26982,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>6</v>
       </c>
@@ -27020,7 +27019,7 @@
       <c r="L31" s="2">
         <v>0</v>
       </c>
-      <c r="M31" s="8">
+      <c r="M31" s="3">
         <v>-3.8163916471489762E-17</v>
       </c>
       <c r="N31" s="2">
@@ -27054,7 +27053,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>7</v>
       </c>
@@ -27091,7 +27090,7 @@
       <c r="L32" s="2">
         <v>0</v>
       </c>
-      <c r="M32" s="8">
+      <c r="M32" s="3">
         <v>0</v>
       </c>
       <c r="N32" s="2">
@@ -27162,7 +27161,7 @@
       <c r="L33" s="2">
         <v>-1.387778780781446E-17</v>
       </c>
-      <c r="M33" s="8">
+      <c r="M33" s="3">
         <v>-1.387778780781446E-17</v>
       </c>
       <c r="N33" s="2">
@@ -27257,9 +27256,8 @@
       <c r="U35">
         <v>19</v>
       </c>
-      <c r="W35" s="6"/>
-      <c r="X35" s="6" t="s">
-        <v>44</v>
+      <c r="V35">
+        <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.3">
@@ -27270,10 +27268,10 @@
         <v>1</v>
       </c>
       <c r="C36" s="2">
-        <v>0.72222222222222343</v>
+        <v>0.50000000000000178</v>
       </c>
       <c r="D36" s="2">
-        <v>0.44444444444444259</v>
+        <v>0</v>
       </c>
       <c r="E36" s="2">
         <v>0</v>
@@ -27294,13 +27292,13 @@
         <v>0</v>
       </c>
       <c r="K36" s="2">
-        <v>4.0708177569589081E-16</v>
+        <v>3.1918911957973251E-16</v>
       </c>
       <c r="L36" s="2">
         <v>0</v>
       </c>
       <c r="M36" s="2">
-        <v>0</v>
+        <v>-1.110223024625157E-16</v>
       </c>
       <c r="N36" s="2">
         <v>0</v>
@@ -27321,164 +27319,167 @@
         <v>0</v>
       </c>
       <c r="T36" s="2">
-        <v>-2.1666666666666661</v>
+        <v>-1.500000000000002</v>
       </c>
       <c r="U36" s="2">
-        <v>0.58333333333333337</v>
+        <v>0.25000000000000128</v>
       </c>
       <c r="V36" s="8">
-        <v>-0.58333333333333337</v>
+        <v>-0.25000000000000128</v>
       </c>
       <c r="W36" s="2">
-        <v>0.99999999999999933</v>
+        <v>1.500000000000002</v>
       </c>
       <c r="Y36">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>11</v>
-      </c>
-      <c r="B37" s="2">
-        <v>0</v>
-      </c>
-      <c r="C37" s="2">
-        <v>2001599834386888</v>
-      </c>
-      <c r="D37" s="2">
-        <v>4003199668773772</v>
-      </c>
-      <c r="E37" s="2">
-        <v>0</v>
-      </c>
-      <c r="F37" s="2">
-        <v>0</v>
-      </c>
-      <c r="G37" s="2">
-        <v>0</v>
-      </c>
-      <c r="H37" s="2">
-        <v>0</v>
-      </c>
-      <c r="I37" s="2">
-        <v>0</v>
-      </c>
-      <c r="J37" s="2">
-        <v>0</v>
-      </c>
-      <c r="K37" s="2">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="L37" s="2">
-        <v>0</v>
-      </c>
-      <c r="M37" s="2">
-        <v>1</v>
-      </c>
-      <c r="N37" s="2">
-        <v>0</v>
-      </c>
-      <c r="O37" s="2">
-        <v>0</v>
-      </c>
-      <c r="P37" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q37" s="2">
-        <v>0</v>
-      </c>
-      <c r="R37" s="2">
-        <v>0</v>
-      </c>
-      <c r="S37" s="2">
-        <v>0</v>
-      </c>
-      <c r="T37" s="2">
-        <v>-6004799503160661</v>
-      </c>
-      <c r="U37" s="2">
-        <v>3002399751580330</v>
+        <v>10</v>
+      </c>
+      <c r="B37" s="8">
+        <v>0</v>
+      </c>
+      <c r="C37" s="8">
+        <v>-2.666666666666667</v>
+      </c>
+      <c r="D37" s="8">
+        <v>0</v>
+      </c>
+      <c r="E37" s="8">
+        <v>0</v>
+      </c>
+      <c r="F37" s="8">
+        <v>0</v>
+      </c>
+      <c r="G37" s="8">
+        <v>0</v>
+      </c>
+      <c r="H37" s="8">
+        <v>0</v>
+      </c>
+      <c r="I37" s="8">
+        <v>0</v>
+      </c>
+      <c r="J37" s="8">
+        <v>0</v>
+      </c>
+      <c r="K37" s="8">
+        <v>-0.50000000000000056</v>
+      </c>
+      <c r="L37" s="8">
+        <v>1</v>
+      </c>
+      <c r="M37" s="8">
+        <v>-0.500000000000001</v>
+      </c>
+      <c r="N37" s="8">
+        <v>0</v>
+      </c>
+      <c r="O37" s="8">
+        <v>0</v>
+      </c>
+      <c r="P37" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="8">
+        <v>0</v>
+      </c>
+      <c r="R37" s="8">
+        <v>0</v>
+      </c>
+      <c r="S37" s="8">
+        <v>0</v>
+      </c>
+      <c r="T37" s="8">
+        <v>2.666666666666667</v>
+      </c>
+      <c r="U37" s="8">
+        <v>-1.833333333333333</v>
       </c>
       <c r="V37" s="8">
-        <v>-3002399751580330</v>
-      </c>
-      <c r="W37" s="2">
-        <v>0</v>
+        <v>1.833333333333333</v>
+      </c>
+      <c r="W37" s="8">
+        <v>-2.666666666666667</v>
+      </c>
+      <c r="X37">
+        <v>-2.666666666666667</v>
       </c>
       <c r="Y37">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>10</v>
       </c>
-      <c r="B38" s="8">
-        <v>0</v>
-      </c>
-      <c r="C38" s="8">
-        <v>1000799917193444</v>
-      </c>
-      <c r="D38" s="8">
-        <v>2001599834386890</v>
-      </c>
-      <c r="E38" s="8">
-        <v>0</v>
-      </c>
-      <c r="F38" s="8">
-        <v>0</v>
-      </c>
-      <c r="G38" s="8">
-        <v>0</v>
-      </c>
-      <c r="H38" s="8">
-        <v>0</v>
-      </c>
-      <c r="I38" s="8">
-        <v>0</v>
-      </c>
-      <c r="J38" s="8">
-        <v>0</v>
-      </c>
-      <c r="K38" s="8">
-        <v>-0.16666666666666649</v>
-      </c>
-      <c r="L38" s="8">
-        <v>1</v>
-      </c>
-      <c r="M38" s="8">
-        <v>0</v>
-      </c>
-      <c r="N38" s="8">
-        <v>0</v>
-      </c>
-      <c r="O38" s="8">
-        <v>0</v>
-      </c>
-      <c r="P38" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q38" s="8">
-        <v>0</v>
-      </c>
-      <c r="R38" s="8">
-        <v>0</v>
-      </c>
-      <c r="S38" s="8">
-        <v>0</v>
-      </c>
-      <c r="T38" s="8">
-        <v>-3002399751580334</v>
-      </c>
-      <c r="U38" s="8">
-        <v>1501199875790167</v>
+      <c r="B38" s="2">
+        <v>0</v>
+      </c>
+      <c r="C38" s="2">
+        <v>0.50000000000000044</v>
+      </c>
+      <c r="D38" s="2">
+        <v>1</v>
+      </c>
+      <c r="E38" s="2">
+        <v>0</v>
+      </c>
+      <c r="F38" s="2">
+        <v>0</v>
+      </c>
+      <c r="G38" s="2">
+        <v>0</v>
+      </c>
+      <c r="H38" s="2">
+        <v>0</v>
+      </c>
+      <c r="I38" s="2">
+        <v>0</v>
+      </c>
+      <c r="J38" s="2">
+        <v>0</v>
+      </c>
+      <c r="K38" s="2">
+        <v>1.6653345369377351E-16</v>
+      </c>
+      <c r="L38" s="2">
+        <v>0</v>
+      </c>
+      <c r="M38" s="2">
+        <v>2.4980018054066022E-16</v>
+      </c>
+      <c r="N38" s="2">
+        <v>0</v>
+      </c>
+      <c r="O38" s="2">
+        <v>0</v>
+      </c>
+      <c r="P38" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q38" s="2">
+        <v>0</v>
+      </c>
+      <c r="R38" s="2">
+        <v>0</v>
+      </c>
+      <c r="S38" s="2">
+        <v>0</v>
+      </c>
+      <c r="T38" s="2">
+        <v>-1.5</v>
+      </c>
+      <c r="U38" s="2">
+        <v>0.75000000000000022</v>
       </c>
       <c r="V38" s="8">
-        <v>-1501199875790167</v>
-      </c>
-      <c r="W38" s="8">
-        <v>1</v>
+        <v>-0.75000000000000022</v>
+      </c>
+      <c r="W38" s="2">
+        <v>1.5</v>
       </c>
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.3">
@@ -27489,10 +27490,10 @@
         <v>0</v>
       </c>
       <c r="C39" s="2">
-        <v>0.1430555555555558</v>
+        <v>0.10000000000000039</v>
       </c>
       <c r="D39" s="2">
-        <v>8.6111111111110708E-2</v>
+        <v>0</v>
       </c>
       <c r="E39" s="2">
         <v>1</v>
@@ -27513,13 +27514,13 @@
         <v>0</v>
       </c>
       <c r="K39" s="2">
-        <v>8.4423209164204608E-17</v>
+        <v>6.7654215563095477E-17</v>
       </c>
       <c r="L39" s="2">
         <v>0</v>
       </c>
       <c r="M39" s="2">
-        <v>0</v>
+        <v>-2.0816681711721691E-17</v>
       </c>
       <c r="N39" s="2">
         <v>-0.5</v>
@@ -27540,16 +27541,16 @@
         <v>0</v>
       </c>
       <c r="T39" s="2">
-        <v>-1.229166666666667</v>
+        <v>-1.100000000000001</v>
       </c>
       <c r="U39" s="2">
-        <v>0.1145833333333333</v>
+        <v>5.0000000000000273E-2</v>
       </c>
       <c r="V39" s="8">
-        <v>-0.1145833333333333</v>
+        <v>-5.0000000000000273E-2</v>
       </c>
       <c r="W39" s="2">
-        <v>0.99999999999999989</v>
+        <v>1.100000000000001</v>
       </c>
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.3">
@@ -27631,10 +27632,10 @@
         <v>0</v>
       </c>
       <c r="C41" s="2">
-        <v>2.7777777777777769E-2</v>
+        <v>0.1</v>
       </c>
       <c r="D41" s="2">
-        <v>-0.14444444444444449</v>
+        <v>0</v>
       </c>
       <c r="E41" s="2">
         <v>0</v>
@@ -27655,13 +27656,13 @@
         <v>0</v>
       </c>
       <c r="K41" s="2">
-        <v>-4.6259292692714861E-18</v>
+        <v>1.387778780781446E-17</v>
       </c>
       <c r="L41" s="2">
-        <v>-1.387778780781446E-17</v>
+        <v>0</v>
       </c>
       <c r="M41" s="2">
-        <v>0</v>
+        <v>4.163336342344337E-17</v>
       </c>
       <c r="N41" s="2">
         <v>0</v>
@@ -27682,16 +27683,16 @@
         <v>0.5</v>
       </c>
       <c r="T41" s="2">
-        <v>-0.88333333333333341</v>
+        <v>-1.1000000000000001</v>
       </c>
       <c r="U41" s="2">
-        <v>4.1666666666666657E-2</v>
+        <v>0.15</v>
       </c>
       <c r="V41" s="8">
-        <v>-4.1666666666666657E-2</v>
+        <v>-0.15</v>
       </c>
       <c r="W41" s="2">
-        <v>0.8</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.3">
@@ -27702,10 +27703,10 @@
         <v>0</v>
       </c>
       <c r="C42" s="2">
-        <v>0.1430555555555558</v>
+        <v>0.10000000000000039</v>
       </c>
       <c r="D42" s="2">
-        <v>8.6111111111110708E-2</v>
+        <v>0</v>
       </c>
       <c r="E42" s="2">
         <v>0</v>
@@ -27726,13 +27727,13 @@
         <v>0</v>
       </c>
       <c r="K42" s="2">
-        <v>8.4423209164204608E-17</v>
+        <v>6.7654215563095477E-17</v>
       </c>
       <c r="L42" s="2">
         <v>0</v>
       </c>
       <c r="M42" s="2">
-        <v>0</v>
+        <v>-2.0816681711721691E-17</v>
       </c>
       <c r="N42" s="2">
         <v>0.5</v>
@@ -27753,16 +27754,16 @@
         <v>0</v>
       </c>
       <c r="T42" s="2">
-        <v>-1.229166666666667</v>
+        <v>-1.100000000000001</v>
       </c>
       <c r="U42" s="2">
-        <v>0.1145833333333333</v>
+        <v>5.0000000000000273E-2</v>
       </c>
       <c r="V42" s="8">
-        <v>-0.1145833333333333</v>
+        <v>-5.0000000000000273E-2</v>
       </c>
       <c r="W42" s="2">
-        <v>0.99999999999999989</v>
+        <v>1.100000000000001</v>
       </c>
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.3">
@@ -27844,10 +27845,10 @@
         <v>0</v>
       </c>
       <c r="C44" s="2">
-        <v>2.7777777777777769E-2</v>
+        <v>0.1</v>
       </c>
       <c r="D44" s="2">
-        <v>-0.14444444444444449</v>
+        <v>0</v>
       </c>
       <c r="E44" s="2">
         <v>0</v>
@@ -27868,13 +27869,13 @@
         <v>1</v>
       </c>
       <c r="K44" s="2">
-        <v>-4.6259292692714861E-18</v>
+        <v>1.387778780781446E-17</v>
       </c>
       <c r="L44" s="2">
-        <v>-1.387778780781446E-17</v>
+        <v>0</v>
       </c>
       <c r="M44" s="2">
-        <v>0</v>
+        <v>4.163336342344337E-17</v>
       </c>
       <c r="N44" s="2">
         <v>0</v>
@@ -27895,16 +27896,16 @@
         <v>-0.5</v>
       </c>
       <c r="T44" s="2">
-        <v>-0.88333333333333341</v>
+        <v>-1.1000000000000001</v>
       </c>
       <c r="U44" s="2">
-        <v>4.1666666666666657E-2</v>
+        <v>0.15</v>
       </c>
       <c r="V44" s="8">
-        <v>-4.1666666666666657E-2</v>
+        <v>-0.15</v>
       </c>
       <c r="W44" s="2">
-        <v>0.8</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.3">
@@ -27968,377 +27969,368 @@
       <c r="U46">
         <v>19</v>
       </c>
-      <c r="X46" s="6" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="47" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>0</v>
       </c>
-      <c r="B47" s="2">
-        <v>1</v>
-      </c>
-      <c r="C47" s="2">
-        <v>0.33333333333333492</v>
-      </c>
-      <c r="D47" s="2">
-        <v>-0.3333333333333357</v>
-      </c>
-      <c r="E47" s="2">
-        <v>0</v>
-      </c>
-      <c r="F47" s="2">
-        <v>0</v>
-      </c>
-      <c r="G47" s="2">
-        <v>0</v>
-      </c>
-      <c r="H47" s="2">
-        <v>0</v>
-      </c>
-      <c r="I47" s="2">
-        <v>0</v>
-      </c>
-      <c r="J47" s="2">
-        <v>0</v>
-      </c>
-      <c r="K47" s="2">
-        <v>4.7184478546569143E-16</v>
-      </c>
-      <c r="L47" s="2">
-        <v>-3.8857805861880439E-16</v>
-      </c>
-      <c r="M47" s="2">
-        <v>0</v>
-      </c>
-      <c r="N47" s="2">
-        <v>0</v>
-      </c>
-      <c r="O47" s="2">
-        <v>0</v>
-      </c>
-      <c r="P47" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q47" s="2">
-        <v>0</v>
-      </c>
-      <c r="R47" s="2">
-        <v>0</v>
-      </c>
-      <c r="S47" s="2">
-        <v>0</v>
-      </c>
-      <c r="T47" s="2">
-        <v>-0.99999999999999889</v>
-      </c>
-      <c r="U47" s="2">
-        <v>0</v>
-      </c>
-      <c r="V47" s="2">
-        <v>0</v>
-      </c>
-      <c r="W47" s="2">
-        <v>0.999999999999999</v>
-      </c>
-      <c r="X47">
-        <v>2.9999999999999831</v>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>0.50000000000000178</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+      <c r="K47">
+        <v>3.1918911957973251E-16</v>
+      </c>
+      <c r="L47">
+        <v>0</v>
+      </c>
+      <c r="M47">
+        <v>-1.110223024625157E-16</v>
+      </c>
+      <c r="N47">
+        <v>0</v>
+      </c>
+      <c r="O47">
+        <v>0</v>
+      </c>
+      <c r="P47">
+        <v>0</v>
+      </c>
+      <c r="Q47">
+        <v>0</v>
+      </c>
+      <c r="R47">
+        <v>0</v>
+      </c>
+      <c r="S47">
+        <v>0</v>
+      </c>
+      <c r="T47">
+        <v>-1.500000000000002</v>
+      </c>
+      <c r="U47">
+        <v>0.25000000000000128</v>
+      </c>
+      <c r="V47">
+        <v>-0.25000000000000128</v>
+      </c>
+      <c r="W47">
+        <v>0.99999999999999922</v>
       </c>
       <c r="Y47">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>11</v>
-      </c>
-      <c r="B48" s="2">
-        <v>0</v>
-      </c>
-      <c r="C48" s="2">
-        <v>3.25</v>
-      </c>
-      <c r="D48" s="2">
-        <v>-4.5</v>
-      </c>
-      <c r="E48" s="2">
-        <v>0</v>
-      </c>
-      <c r="F48" s="2">
-        <v>0</v>
-      </c>
-      <c r="G48" s="2">
-        <v>0</v>
-      </c>
-      <c r="H48" s="2">
-        <v>0</v>
-      </c>
-      <c r="I48" s="2">
-        <v>0</v>
-      </c>
-      <c r="J48" s="2">
-        <v>0</v>
-      </c>
-      <c r="K48" s="2">
-        <v>0.99999999999999922</v>
-      </c>
-      <c r="L48" s="2">
-        <v>-1.999999999999998</v>
-      </c>
-      <c r="M48" s="2">
-        <v>1</v>
-      </c>
-      <c r="N48" s="2">
-        <v>0</v>
-      </c>
-      <c r="O48" s="2">
-        <v>0</v>
-      </c>
-      <c r="P48" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q48" s="2">
-        <v>0</v>
-      </c>
-      <c r="R48" s="2">
-        <v>0</v>
-      </c>
-      <c r="S48" s="2">
-        <v>0</v>
-      </c>
-      <c r="T48" s="2">
-        <v>2</v>
-      </c>
-      <c r="U48" s="2">
-        <v>0</v>
-      </c>
-      <c r="V48" s="2">
-        <v>0</v>
-      </c>
-      <c r="W48" s="2">
-        <v>-1.999999999999998</v>
+        <v>10</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <v>-2.666666666666667</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+      <c r="K48">
+        <v>-0.50000000000000056</v>
+      </c>
+      <c r="L48">
+        <v>1</v>
+      </c>
+      <c r="M48">
+        <v>-0.500000000000001</v>
+      </c>
+      <c r="N48">
+        <v>0</v>
+      </c>
+      <c r="O48">
+        <v>0</v>
+      </c>
+      <c r="P48">
+        <v>0</v>
+      </c>
+      <c r="Q48">
+        <v>0</v>
+      </c>
+      <c r="R48">
+        <v>0</v>
+      </c>
+      <c r="S48">
+        <v>0</v>
+      </c>
+      <c r="T48">
+        <v>2.666666666666667</v>
+      </c>
+      <c r="U48">
+        <v>-1.833333333333333</v>
+      </c>
+      <c r="V48">
+        <v>1.833333333333333</v>
+      </c>
+      <c r="W48">
+        <v>0.99999999999999911</v>
       </c>
       <c r="X48">
-        <v>-0.61538461538461475</v>
+        <v>0.54545454545454508</v>
       </c>
       <c r="Y48">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="49" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>20</v>
-      </c>
-      <c r="B49" s="2">
-        <v>0</v>
-      </c>
-      <c r="C49" s="2">
-        <v>-0.66666666666666596</v>
-      </c>
-      <c r="D49" s="2">
-        <v>-1.3333333333333339</v>
-      </c>
-      <c r="E49" s="2">
-        <v>0</v>
-      </c>
-      <c r="F49" s="2">
-        <v>0</v>
-      </c>
-      <c r="G49" s="2">
-        <v>0</v>
-      </c>
-      <c r="H49" s="2">
-        <v>0</v>
-      </c>
-      <c r="I49" s="2">
-        <v>0</v>
-      </c>
-      <c r="J49" s="2">
-        <v>0</v>
-      </c>
-      <c r="K49" s="2">
-        <v>1.110223024625154E-16</v>
-      </c>
-      <c r="L49" s="2">
-        <v>-6.6613381477509333E-16</v>
-      </c>
-      <c r="M49" s="2">
-        <v>0</v>
-      </c>
-      <c r="N49" s="2">
-        <v>0</v>
-      </c>
-      <c r="O49" s="2">
-        <v>0</v>
-      </c>
-      <c r="P49" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q49" s="2">
-        <v>0</v>
-      </c>
-      <c r="R49" s="2">
-        <v>0</v>
-      </c>
-      <c r="S49" s="2">
-        <v>0</v>
-      </c>
-      <c r="T49" s="2">
-        <v>2</v>
-      </c>
-      <c r="U49" s="2">
-        <v>-1</v>
-      </c>
-      <c r="V49" s="2">
-        <v>1</v>
-      </c>
-      <c r="W49" s="2">
-        <v>-6.6613381477509333E-16</v>
+        <v>10</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+      <c r="C49">
+        <v>0.50000000000000044</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49">
+        <v>0</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+      <c r="K49">
+        <v>1.6653345369377351E-16</v>
+      </c>
+      <c r="L49">
+        <v>0</v>
+      </c>
+      <c r="M49">
+        <v>2.4980018054066022E-16</v>
+      </c>
+      <c r="N49">
+        <v>0</v>
+      </c>
+      <c r="O49">
+        <v>0</v>
+      </c>
+      <c r="P49">
+        <v>0</v>
+      </c>
+      <c r="Q49">
+        <v>0</v>
+      </c>
+      <c r="R49">
+        <v>0</v>
+      </c>
+      <c r="S49">
+        <v>0</v>
+      </c>
+      <c r="T49">
+        <v>-1.5</v>
+      </c>
+      <c r="U49">
+        <v>0.75000000000000022</v>
+      </c>
+      <c r="V49">
+        <v>-0.75000000000000022</v>
+      </c>
+      <c r="W49">
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>3</v>
       </c>
-      <c r="B50" s="2">
-        <v>0</v>
-      </c>
-      <c r="C50" s="2">
-        <v>6.6666666666666985E-2</v>
-      </c>
-      <c r="D50" s="2">
-        <v>-6.6666666666667193E-2</v>
-      </c>
-      <c r="E50" s="2">
-        <v>1</v>
-      </c>
-      <c r="F50" s="2">
-        <v>0</v>
-      </c>
-      <c r="G50" s="2">
-        <v>0</v>
-      </c>
-      <c r="H50" s="2">
-        <v>0</v>
-      </c>
-      <c r="I50" s="2">
-        <v>0</v>
-      </c>
-      <c r="J50" s="2">
-        <v>0</v>
-      </c>
-      <c r="K50" s="2">
-        <v>9.7144514654701173E-17</v>
-      </c>
-      <c r="L50" s="2">
-        <v>-7.6327832942979438E-17</v>
-      </c>
-      <c r="M50" s="2">
-        <v>0</v>
-      </c>
-      <c r="N50" s="2">
+      <c r="B50">
+        <v>0</v>
+      </c>
+      <c r="C50">
+        <v>0.10000000000000039</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <v>0</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
+      <c r="K50">
+        <v>6.7654215563095477E-17</v>
+      </c>
+      <c r="L50">
+        <v>0</v>
+      </c>
+      <c r="M50">
+        <v>-2.0816681711721691E-17</v>
+      </c>
+      <c r="N50">
         <v>-0.5</v>
       </c>
-      <c r="O50" s="2">
+      <c r="O50">
         <v>0.5</v>
       </c>
-      <c r="P50" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q50" s="2">
+      <c r="P50">
+        <v>0</v>
+      </c>
+      <c r="Q50">
         <v>0.5</v>
       </c>
-      <c r="R50" s="2">
+      <c r="R50">
         <v>-0.5</v>
       </c>
-      <c r="S50" s="2">
-        <v>0</v>
-      </c>
-      <c r="T50" s="2">
-        <v>-0.99999999999999978</v>
-      </c>
-      <c r="U50" s="2">
-        <v>-1.387778780781446E-17</v>
-      </c>
-      <c r="V50" s="2">
-        <v>1.387778780781446E-17</v>
-      </c>
-      <c r="W50" s="2">
-        <v>0.99999999999999978</v>
-      </c>
-      <c r="X50">
-        <v>14.999999999999931</v>
+      <c r="S50">
+        <v>0</v>
+      </c>
+      <c r="T50">
+        <v>-1.100000000000001</v>
+      </c>
+      <c r="U50">
+        <v>5.0000000000000273E-2</v>
+      </c>
+      <c r="V50">
+        <v>-5.0000000000000273E-2</v>
+      </c>
+      <c r="W50">
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>4</v>
       </c>
-      <c r="B51" s="2">
-        <v>0</v>
-      </c>
-      <c r="C51" s="2">
+      <c r="B51">
+        <v>0</v>
+      </c>
+      <c r="C51">
         <v>-0.2</v>
       </c>
-      <c r="D51" s="2">
-        <v>0</v>
-      </c>
-      <c r="E51" s="2">
-        <v>0</v>
-      </c>
-      <c r="F51" s="2">
-        <v>1</v>
-      </c>
-      <c r="G51" s="2">
-        <v>0</v>
-      </c>
-      <c r="H51" s="2">
-        <v>0</v>
-      </c>
-      <c r="I51" s="2">
-        <v>0</v>
-      </c>
-      <c r="J51" s="2">
-        <v>0</v>
-      </c>
-      <c r="K51" s="2">
-        <v>0</v>
-      </c>
-      <c r="L51" s="2">
-        <v>0</v>
-      </c>
-      <c r="M51" s="2">
-        <v>0</v>
-      </c>
-      <c r="N51" s="2">
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <v>1</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+      <c r="I51">
+        <v>0</v>
+      </c>
+      <c r="J51">
+        <v>0</v>
+      </c>
+      <c r="K51">
+        <v>0</v>
+      </c>
+      <c r="L51">
+        <v>0</v>
+      </c>
+      <c r="M51">
+        <v>0</v>
+      </c>
+      <c r="N51">
         <v>0.5</v>
       </c>
-      <c r="O51" s="2">
+      <c r="O51">
         <v>-1</v>
       </c>
-      <c r="P51" s="2">
+      <c r="P51">
         <v>0.5</v>
       </c>
-      <c r="Q51" s="2">
+      <c r="Q51">
         <v>-0.5</v>
       </c>
-      <c r="R51" s="2">
-        <v>1</v>
-      </c>
-      <c r="S51" s="2">
+      <c r="R51">
+        <v>1</v>
+      </c>
+      <c r="S51">
         <v>-0.5</v>
       </c>
-      <c r="T51" s="2">
+      <c r="T51">
         <v>-0.8</v>
       </c>
-      <c r="U51" s="2">
-        <v>0</v>
-      </c>
-      <c r="V51" s="2">
-        <v>0</v>
-      </c>
-      <c r="W51" s="2">
+      <c r="U51">
+        <v>0</v>
+      </c>
+      <c r="V51">
+        <v>0</v>
+      </c>
+      <c r="W51">
         <v>0.8</v>
       </c>
     </row>
@@ -28346,218 +28338,212 @@
       <c r="A52">
         <v>5</v>
       </c>
-      <c r="B52" s="2">
-        <v>0</v>
-      </c>
-      <c r="C52" s="2">
-        <v>1.7347234759768071E-17</v>
-      </c>
-      <c r="D52" s="2">
-        <v>-0.20000000000000009</v>
-      </c>
-      <c r="E52" s="2">
-        <v>0</v>
-      </c>
-      <c r="F52" s="2">
-        <v>0</v>
-      </c>
-      <c r="G52" s="2">
-        <v>1</v>
-      </c>
-      <c r="H52" s="2">
-        <v>0</v>
-      </c>
-      <c r="I52" s="2">
-        <v>0</v>
-      </c>
-      <c r="J52" s="2">
-        <v>0</v>
-      </c>
-      <c r="K52" s="2">
-        <v>-1.0785207688568519E-32</v>
-      </c>
-      <c r="L52" s="2">
-        <v>-4.1633363423443352E-17</v>
-      </c>
-      <c r="M52" s="2">
-        <v>0</v>
-      </c>
-      <c r="N52" s="2">
-        <v>0</v>
-      </c>
-      <c r="O52" s="2">
+      <c r="B52">
+        <v>0</v>
+      </c>
+      <c r="C52">
+        <v>0.1</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52">
+        <v>0</v>
+      </c>
+      <c r="G52">
+        <v>1</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+      <c r="I52">
+        <v>0</v>
+      </c>
+      <c r="J52">
+        <v>0</v>
+      </c>
+      <c r="K52">
+        <v>1.387778780781446E-17</v>
+      </c>
+      <c r="L52">
+        <v>0</v>
+      </c>
+      <c r="M52">
+        <v>4.163336342344337E-17</v>
+      </c>
+      <c r="N52">
+        <v>0</v>
+      </c>
+      <c r="O52">
         <v>0.5</v>
       </c>
-      <c r="P52" s="2">
+      <c r="P52">
         <v>-0.5</v>
       </c>
-      <c r="Q52" s="2">
-        <v>0</v>
-      </c>
-      <c r="R52" s="2">
+      <c r="Q52">
+        <v>0</v>
+      </c>
+      <c r="R52">
         <v>-0.5</v>
       </c>
-      <c r="S52" s="2">
+      <c r="S52">
         <v>0.5</v>
       </c>
-      <c r="T52" s="2">
-        <v>-0.8</v>
-      </c>
-      <c r="U52" s="2">
-        <v>0</v>
-      </c>
-      <c r="V52" s="2">
-        <v>0</v>
-      </c>
-      <c r="W52" s="2">
+      <c r="T52">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="U52">
+        <v>0.15</v>
+      </c>
+      <c r="V52">
+        <v>-0.15</v>
+      </c>
+      <c r="W52">
         <v>0.8</v>
-      </c>
-      <c r="X52">
-        <v>4.611686018427388E+16</v>
       </c>
     </row>
     <row r="53" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>6</v>
       </c>
-      <c r="B53" s="2">
-        <v>0</v>
-      </c>
-      <c r="C53" s="2">
-        <v>6.6666666666666985E-2</v>
-      </c>
-      <c r="D53" s="2">
-        <v>-6.6666666666667193E-2</v>
-      </c>
-      <c r="E53" s="2">
-        <v>0</v>
-      </c>
-      <c r="F53" s="2">
-        <v>0</v>
-      </c>
-      <c r="G53" s="2">
-        <v>0</v>
-      </c>
-      <c r="H53" s="2">
-        <v>1</v>
-      </c>
-      <c r="I53" s="2">
-        <v>0</v>
-      </c>
-      <c r="J53" s="2">
-        <v>0</v>
-      </c>
-      <c r="K53" s="2">
-        <v>9.7144514654701173E-17</v>
-      </c>
-      <c r="L53" s="2">
-        <v>-7.6327832942979438E-17</v>
-      </c>
-      <c r="M53" s="2">
-        <v>0</v>
-      </c>
-      <c r="N53" s="2">
+      <c r="B53">
+        <v>0</v>
+      </c>
+      <c r="C53">
+        <v>0.10000000000000039</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <v>1</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+      <c r="J53">
+        <v>0</v>
+      </c>
+      <c r="K53">
+        <v>6.7654215563095477E-17</v>
+      </c>
+      <c r="L53">
+        <v>0</v>
+      </c>
+      <c r="M53">
+        <v>-2.0816681711721691E-17</v>
+      </c>
+      <c r="N53">
         <v>0.5</v>
       </c>
-      <c r="O53" s="2">
+      <c r="O53">
         <v>-0.5</v>
       </c>
-      <c r="P53" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q53" s="2">
+      <c r="P53">
+        <v>0</v>
+      </c>
+      <c r="Q53">
         <v>-0.5</v>
       </c>
-      <c r="R53" s="2">
+      <c r="R53">
         <v>0.5</v>
       </c>
-      <c r="S53" s="2">
-        <v>0</v>
-      </c>
-      <c r="T53" s="2">
-        <v>-0.99999999999999978</v>
-      </c>
-      <c r="U53" s="2">
-        <v>-1.387778780781446E-17</v>
-      </c>
-      <c r="V53" s="2">
-        <v>1.387778780781446E-17</v>
-      </c>
-      <c r="W53" s="2">
-        <v>0.99999999999999978</v>
-      </c>
-      <c r="X53">
-        <v>14.999999999999931</v>
+      <c r="S53">
+        <v>0</v>
+      </c>
+      <c r="T53">
+        <v>-1.100000000000001</v>
+      </c>
+      <c r="U53">
+        <v>5.0000000000000273E-2</v>
+      </c>
+      <c r="V53">
+        <v>-5.0000000000000273E-2</v>
+      </c>
+      <c r="W53">
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>7</v>
       </c>
-      <c r="B54" s="2">
-        <v>0</v>
-      </c>
-      <c r="C54" s="2">
+      <c r="B54">
+        <v>0</v>
+      </c>
+      <c r="C54">
         <v>-0.2</v>
       </c>
-      <c r="D54" s="2">
-        <v>0</v>
-      </c>
-      <c r="E54" s="2">
-        <v>0</v>
-      </c>
-      <c r="F54" s="2">
-        <v>0</v>
-      </c>
-      <c r="G54" s="2">
-        <v>0</v>
-      </c>
-      <c r="H54" s="2">
-        <v>0</v>
-      </c>
-      <c r="I54" s="2">
-        <v>1</v>
-      </c>
-      <c r="J54" s="2">
-        <v>0</v>
-      </c>
-      <c r="K54" s="2">
-        <v>0</v>
-      </c>
-      <c r="L54" s="2">
-        <v>0</v>
-      </c>
-      <c r="M54" s="2">
-        <v>0</v>
-      </c>
-      <c r="N54" s="2">
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+      <c r="I54">
+        <v>1</v>
+      </c>
+      <c r="J54">
+        <v>0</v>
+      </c>
+      <c r="K54">
+        <v>0</v>
+      </c>
+      <c r="L54">
+        <v>0</v>
+      </c>
+      <c r="M54">
+        <v>0</v>
+      </c>
+      <c r="N54">
         <v>-0.5</v>
       </c>
-      <c r="O54" s="2">
-        <v>1</v>
-      </c>
-      <c r="P54" s="2">
+      <c r="O54">
+        <v>1</v>
+      </c>
+      <c r="P54">
         <v>-0.5</v>
       </c>
-      <c r="Q54" s="2">
+      <c r="Q54">
         <v>0.5</v>
       </c>
-      <c r="R54" s="2">
+      <c r="R54">
         <v>-1</v>
       </c>
-      <c r="S54" s="2">
+      <c r="S54">
         <v>0.5</v>
       </c>
-      <c r="T54" s="2">
+      <c r="T54">
         <v>-0.8</v>
       </c>
-      <c r="U54" s="2">
-        <v>0</v>
-      </c>
-      <c r="V54" s="2">
-        <v>0</v>
-      </c>
-      <c r="W54" s="2">
+      <c r="U54">
+        <v>0</v>
+      </c>
+      <c r="V54">
+        <v>0</v>
+      </c>
+      <c r="W54">
         <v>0.8</v>
       </c>
     </row>
@@ -28565,74 +28551,71 @@
       <c r="A55">
         <v>8</v>
       </c>
-      <c r="B55" s="2">
-        <v>0</v>
-      </c>
-      <c r="C55" s="2">
-        <v>1.7347234759768071E-17</v>
-      </c>
-      <c r="D55" s="2">
-        <v>-0.20000000000000009</v>
-      </c>
-      <c r="E55" s="2">
-        <v>0</v>
-      </c>
-      <c r="F55" s="2">
-        <v>0</v>
-      </c>
-      <c r="G55" s="2">
-        <v>0</v>
-      </c>
-      <c r="H55" s="2">
-        <v>0</v>
-      </c>
-      <c r="I55" s="2">
-        <v>0</v>
-      </c>
-      <c r="J55" s="2">
-        <v>1</v>
-      </c>
-      <c r="K55" s="2">
-        <v>-1.0785207688568519E-32</v>
-      </c>
-      <c r="L55" s="2">
-        <v>-4.1633363423443352E-17</v>
-      </c>
-      <c r="M55" s="2">
-        <v>0</v>
-      </c>
-      <c r="N55" s="2">
-        <v>0</v>
-      </c>
-      <c r="O55" s="2">
+      <c r="B55">
+        <v>0</v>
+      </c>
+      <c r="C55">
+        <v>0.1</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
+      <c r="I55">
+        <v>0</v>
+      </c>
+      <c r="J55">
+        <v>1</v>
+      </c>
+      <c r="K55">
+        <v>1.387778780781446E-17</v>
+      </c>
+      <c r="L55">
+        <v>0</v>
+      </c>
+      <c r="M55">
+        <v>4.163336342344337E-17</v>
+      </c>
+      <c r="N55">
+        <v>0</v>
+      </c>
+      <c r="O55">
         <v>-0.5</v>
       </c>
-      <c r="P55" s="2">
+      <c r="P55">
         <v>0.5</v>
       </c>
-      <c r="Q55" s="2">
-        <v>0</v>
-      </c>
-      <c r="R55" s="2">
+      <c r="Q55">
+        <v>0</v>
+      </c>
+      <c r="R55">
         <v>0.5</v>
       </c>
-      <c r="S55" s="2">
+      <c r="S55">
         <v>-0.5</v>
       </c>
-      <c r="T55" s="2">
-        <v>-0.8</v>
-      </c>
-      <c r="U55" s="2">
-        <v>0</v>
-      </c>
-      <c r="V55" s="2">
-        <v>0</v>
-      </c>
-      <c r="W55" s="2">
+      <c r="T55">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="U55">
+        <v>0.15</v>
+      </c>
+      <c r="V55">
+        <v>-0.15</v>
+      </c>
+      <c r="W55">
         <v>0.8</v>
-      </c>
-      <c r="X55">
-        <v>4.611686018427388E+16</v>
       </c>
     </row>
     <row r="57" spans="1:25" x14ac:dyDescent="0.3">
@@ -28699,16 +28682,16 @@
     </row>
     <row r="58" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B58">
-        <v>2.9999999999999858</v>
+        <v>1</v>
       </c>
       <c r="C58">
-        <v>1</v>
+        <v>0.13636363636363619</v>
       </c>
       <c r="D58">
-        <v>-1.000000000000002</v>
+        <v>0</v>
       </c>
       <c r="E58">
         <v>0</v>
@@ -28729,13 +28712,13 @@
         <v>0</v>
       </c>
       <c r="K58">
-        <v>1.4155343563970671E-15</v>
+        <v>-6.8181818181818302E-2</v>
       </c>
       <c r="L58">
-        <v>-1.1657341758564081E-15</v>
+        <v>0.1363636363636371</v>
       </c>
       <c r="M58">
-        <v>0</v>
+        <v>-6.8181818181818787E-2</v>
       </c>
       <c r="N58">
         <v>0</v>
@@ -28756,7 +28739,7 @@
         <v>0</v>
       </c>
       <c r="T58">
-        <v>-2.9999999999999818</v>
+        <v>-1.136363636363636</v>
       </c>
       <c r="U58">
         <v>0</v>
@@ -28765,27 +28748,27 @@
         <v>0</v>
       </c>
       <c r="W58">
-        <v>2.9999999999999831</v>
+        <v>1.136363636363636</v>
       </c>
       <c r="X58">
-        <v>2119341001115526</v>
+        <v>8.3333333333333428</v>
       </c>
       <c r="Y58">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A59">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B59">
-        <v>-9.7499999999999538</v>
+        <v>0</v>
       </c>
       <c r="C59">
-        <v>-4.4408920985006262E-16</v>
+        <v>-1.454545454545455</v>
       </c>
       <c r="D59">
-        <v>-1.249999999999992</v>
+        <v>0</v>
       </c>
       <c r="E59">
         <v>0</v>
@@ -28806,13 +28789,13 @@
         <v>0</v>
       </c>
       <c r="K59">
-        <v>0.99999999999999467</v>
+        <v>-0.2727272727272731</v>
       </c>
       <c r="L59">
-        <v>-1.999999999999994</v>
+        <v>0.54545454545454553</v>
       </c>
       <c r="M59">
-        <v>1</v>
+        <v>-0.27272727272727332</v>
       </c>
       <c r="N59">
         <v>0</v>
@@ -28833,36 +28816,33 @@
         <v>0</v>
       </c>
       <c r="T59">
-        <v>11.74999999999994</v>
+        <v>1.454545454545455</v>
       </c>
       <c r="U59">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="V59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W59">
-        <v>-11.74999999999994</v>
-      </c>
-      <c r="X59">
-        <v>-11.750000000000011</v>
+        <v>0.54545454545454508</v>
       </c>
       <c r="Y59">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A60">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B60">
-        <v>1.999999999999988</v>
+        <v>0</v>
       </c>
       <c r="C60">
-        <v>0</v>
+        <v>-0.59090909090909105</v>
       </c>
       <c r="D60">
-        <v>-2.0000000000000022</v>
+        <v>1</v>
       </c>
       <c r="E60">
         <v>0</v>
@@ -28883,13 +28863,13 @@
         <v>0</v>
       </c>
       <c r="K60">
-        <v>1.054711873393893E-15</v>
+        <v>-0.2045454545454547</v>
       </c>
       <c r="L60">
-        <v>-1.443289932012698E-15</v>
+        <v>0.40909090909090928</v>
       </c>
       <c r="M60">
-        <v>0</v>
+        <v>-0.20454545454545481</v>
       </c>
       <c r="N60">
         <v>0</v>
@@ -28910,19 +28890,16 @@
         <v>0</v>
       </c>
       <c r="T60">
-        <v>1.4432899320127041E-14</v>
+        <v>-0.40909090909090889</v>
       </c>
       <c r="U60">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="V60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W60">
-        <v>1.999999999999986</v>
-      </c>
-      <c r="X60">
-        <v>1896252474682311</v>
+        <v>0.40909090909090889</v>
       </c>
     </row>
     <row r="61" spans="1:25" x14ac:dyDescent="0.3">
@@ -28930,13 +28907,13 @@
         <v>3</v>
       </c>
       <c r="B61">
-        <v>-0.2</v>
+        <v>0</v>
       </c>
       <c r="C61">
-        <v>0</v>
+        <v>2.727272727272724E-2</v>
       </c>
       <c r="D61">
-        <v>-5.5511151231257827E-17</v>
+        <v>0</v>
       </c>
       <c r="E61">
         <v>1</v>
@@ -28957,13 +28934,13 @@
         <v>0</v>
       </c>
       <c r="K61">
-        <v>2.7755575615628938E-18</v>
+        <v>-1.363636363636366E-2</v>
       </c>
       <c r="L61">
-        <v>1.3877787807814531E-18</v>
+        <v>2.7272727272727431E-2</v>
       </c>
       <c r="M61">
-        <v>0</v>
+        <v>-1.3636363636363761E-2</v>
       </c>
       <c r="N61">
         <v>-0.5</v>
@@ -28984,19 +28961,19 @@
         <v>0</v>
       </c>
       <c r="T61">
-        <v>-0.8</v>
+        <v>-1.0272727272727269</v>
       </c>
       <c r="U61">
-        <v>-1.387778780781446E-17</v>
+        <v>-6.9388939039072284E-18</v>
       </c>
       <c r="V61">
-        <v>1.387778780781446E-17</v>
+        <v>6.9388939039072284E-18</v>
       </c>
       <c r="W61">
-        <v>0.8</v>
+        <v>1.0272727272727269</v>
       </c>
       <c r="X61">
-        <v>2.8823037615171149E+17</v>
+        <v>37.666666666666707</v>
       </c>
     </row>
     <row r="62" spans="1:25" x14ac:dyDescent="0.3">
@@ -29004,13 +28981,13 @@
         <v>4</v>
       </c>
       <c r="B62">
-        <v>0.5999999999999972</v>
+        <v>0</v>
       </c>
       <c r="C62">
-        <v>0</v>
+        <v>-0.2</v>
       </c>
       <c r="D62">
-        <v>-0.20000000000000051</v>
+        <v>0</v>
       </c>
       <c r="E62">
         <v>0</v>
@@ -29031,10 +29008,10 @@
         <v>0</v>
       </c>
       <c r="K62">
-        <v>2.8310687127941352E-16</v>
+        <v>0</v>
       </c>
       <c r="L62">
-        <v>-2.331468351712816E-16</v>
+        <v>0</v>
       </c>
       <c r="M62">
         <v>0</v>
@@ -29058,7 +29035,7 @@
         <v>-0.5</v>
       </c>
       <c r="T62">
-        <v>-1.399999999999997</v>
+        <v>-0.8</v>
       </c>
       <c r="U62">
         <v>0</v>
@@ -29067,10 +29044,7 @@
         <v>0</v>
       </c>
       <c r="W62">
-        <v>1.399999999999997</v>
-      </c>
-      <c r="X62">
-        <v>4945129002602910</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="63" spans="1:25" x14ac:dyDescent="0.3">
@@ -29078,13 +29052,13 @@
         <v>5</v>
       </c>
       <c r="B63">
-        <v>-5.2041704279303972E-17</v>
+        <v>0</v>
       </c>
       <c r="C63">
-        <v>0</v>
+        <v>-0.11818181818181819</v>
       </c>
       <c r="D63">
-        <v>-0.2</v>
+        <v>0</v>
       </c>
       <c r="E63">
         <v>0</v>
@@ -29105,13 +29079,13 @@
         <v>0</v>
       </c>
       <c r="K63">
-        <v>-3.5340814479505657E-32</v>
+        <v>-4.090909090909095E-2</v>
       </c>
       <c r="L63">
-        <v>-4.1633363423443327E-17</v>
+        <v>8.1818181818181845E-2</v>
       </c>
       <c r="M63">
-        <v>0</v>
+        <v>-4.0909090909090957E-2</v>
       </c>
       <c r="N63">
         <v>0</v>
@@ -29132,16 +29106,16 @@
         <v>0.5</v>
       </c>
       <c r="T63">
-        <v>-0.8</v>
+        <v>-0.88181818181818183</v>
       </c>
       <c r="U63">
-        <v>0</v>
+        <v>-2.775557561562891E-17</v>
       </c>
       <c r="V63">
-        <v>0</v>
+        <v>2.775557561562891E-17</v>
       </c>
       <c r="W63">
-        <v>0.8</v>
+        <v>0.88181818181818183</v>
       </c>
     </row>
     <row r="64" spans="1:25" x14ac:dyDescent="0.3">
@@ -29149,13 +29123,13 @@
         <v>6</v>
       </c>
       <c r="B64">
-        <v>-0.2</v>
+        <v>0</v>
       </c>
       <c r="C64">
-        <v>0</v>
+        <v>2.727272727272724E-2</v>
       </c>
       <c r="D64">
-        <v>-5.5511151231257827E-17</v>
+        <v>0</v>
       </c>
       <c r="E64">
         <v>0</v>
@@ -29176,13 +29150,13 @@
         <v>0</v>
       </c>
       <c r="K64">
-        <v>2.7755575615628938E-18</v>
+        <v>-1.363636363636366E-2</v>
       </c>
       <c r="L64">
-        <v>1.3877787807814531E-18</v>
+        <v>2.7272727272727431E-2</v>
       </c>
       <c r="M64">
-        <v>0</v>
+        <v>-1.3636363636363761E-2</v>
       </c>
       <c r="N64">
         <v>0.5</v>
@@ -29203,19 +29177,19 @@
         <v>0</v>
       </c>
       <c r="T64">
-        <v>-0.8</v>
+        <v>-1.0272727272727269</v>
       </c>
       <c r="U64">
-        <v>-1.387778780781446E-17</v>
+        <v>-6.9388939039072284E-18</v>
       </c>
       <c r="V64">
-        <v>1.387778780781446E-17</v>
+        <v>6.9388939039072284E-18</v>
       </c>
       <c r="W64">
-        <v>0.8</v>
+        <v>1.0272727272727269</v>
       </c>
       <c r="X64">
-        <v>2.8823037615171149E+17</v>
+        <v>37.666666666666707</v>
       </c>
     </row>
     <row r="65" spans="1:25" x14ac:dyDescent="0.3">
@@ -29223,13 +29197,13 @@
         <v>7</v>
       </c>
       <c r="B65">
-        <v>0.5999999999999972</v>
+        <v>0</v>
       </c>
       <c r="C65">
-        <v>0</v>
+        <v>-0.2</v>
       </c>
       <c r="D65">
-        <v>-0.20000000000000051</v>
+        <v>0</v>
       </c>
       <c r="E65">
         <v>0</v>
@@ -29250,10 +29224,10 @@
         <v>0</v>
       </c>
       <c r="K65">
-        <v>2.8310687127941352E-16</v>
+        <v>0</v>
       </c>
       <c r="L65">
-        <v>-2.331468351712816E-16</v>
+        <v>0</v>
       </c>
       <c r="M65">
         <v>0</v>
@@ -29277,7 +29251,7 @@
         <v>0.5</v>
       </c>
       <c r="T65">
-        <v>-1.399999999999997</v>
+        <v>-0.8</v>
       </c>
       <c r="U65">
         <v>0</v>
@@ -29286,10 +29260,7 @@
         <v>0</v>
       </c>
       <c r="W65">
-        <v>1.399999999999997</v>
-      </c>
-      <c r="X65">
-        <v>4945129002602910</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="66" spans="1:25" x14ac:dyDescent="0.3">
@@ -29297,13 +29268,13 @@
         <v>8</v>
       </c>
       <c r="B66">
-        <v>-5.2041704279303972E-17</v>
+        <v>0</v>
       </c>
       <c r="C66">
-        <v>0</v>
+        <v>-0.11818181818181819</v>
       </c>
       <c r="D66">
-        <v>-0.2</v>
+        <v>0</v>
       </c>
       <c r="E66">
         <v>0</v>
@@ -29324,13 +29295,13 @@
         <v>1</v>
       </c>
       <c r="K66">
-        <v>-3.5340814479505657E-32</v>
+        <v>-4.090909090909095E-2</v>
       </c>
       <c r="L66">
-        <v>-4.1633363423443327E-17</v>
+        <v>8.1818181818181845E-2</v>
       </c>
       <c r="M66">
-        <v>0</v>
+        <v>-4.0909090909090957E-2</v>
       </c>
       <c r="N66">
         <v>0</v>
@@ -29351,16 +29322,16 @@
         <v>-0.5</v>
       </c>
       <c r="T66">
-        <v>-0.8</v>
+        <v>-0.88181818181818183</v>
       </c>
       <c r="U66">
-        <v>0</v>
+        <v>-2.775557561562891E-17</v>
       </c>
       <c r="V66">
-        <v>0</v>
+        <v>2.775557561562891E-17</v>
       </c>
       <c r="W66">
-        <v>0.8</v>
+        <v>0.88181818181818183</v>
       </c>
     </row>
     <row r="68" spans="1:25" x14ac:dyDescent="0.3">
@@ -29430,13 +29401,13 @@
         <v>1</v>
       </c>
       <c r="B69">
-        <v>0.31578947368421018</v>
+        <v>7.3333333333333428</v>
       </c>
       <c r="C69">
         <v>1</v>
       </c>
       <c r="D69">
-        <v>1.6842105263157909</v>
+        <v>0</v>
       </c>
       <c r="E69">
         <v>0</v>
@@ -29457,13 +29428,13 @@
         <v>0</v>
       </c>
       <c r="K69">
-        <v>0</v>
+        <v>-0.50000000000000155</v>
       </c>
       <c r="L69">
-        <v>7.7131283816063471E-16</v>
+        <v>1.000000000000006</v>
       </c>
       <c r="M69">
-        <v>0</v>
+        <v>-0.50000000000000511</v>
       </c>
       <c r="N69">
         <v>0</v>
@@ -29484,33 +29455,33 @@
         <v>0</v>
       </c>
       <c r="T69">
-        <v>-3.0000000000000022</v>
+        <v>-8.3333333333333428</v>
       </c>
       <c r="U69">
-        <v>1.342105263157896</v>
+        <v>0</v>
       </c>
       <c r="V69">
-        <v>-1.342105263157896</v>
+        <v>0</v>
       </c>
       <c r="W69">
-        <v>0.31578947368421062</v>
+        <v>8.3333333333333428</v>
       </c>
       <c r="Y69">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A70">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B70">
-        <v>-1896252474682314</v>
+        <v>10.66666666666668</v>
       </c>
       <c r="C70">
-        <v>-4.4408920985006262E-16</v>
+        <v>0</v>
       </c>
       <c r="D70">
-        <v>1896252474682315</v>
+        <v>0</v>
       </c>
       <c r="E70">
         <v>0</v>
@@ -29531,13 +29502,13 @@
         <v>0</v>
       </c>
       <c r="K70">
-        <v>-1.110223024625157E-16</v>
+        <v>-1.0000000000000031</v>
       </c>
       <c r="L70">
-        <v>-0.63157894736842057</v>
+        <v>2.0000000000000102</v>
       </c>
       <c r="M70">
-        <v>1</v>
+        <v>-1.000000000000008</v>
       </c>
       <c r="N70">
         <v>0</v>
@@ -29558,36 +29529,33 @@
         <v>0</v>
       </c>
       <c r="T70">
-        <v>-1.934210526315852</v>
+        <v>-10.66666666666668</v>
       </c>
       <c r="U70">
-        <v>948126237341157.38</v>
+        <v>-1</v>
       </c>
       <c r="V70">
-        <v>-948126237341157.38</v>
+        <v>1</v>
       </c>
       <c r="W70">
-        <v>-1896252474682313</v>
-      </c>
-      <c r="X70">
-        <v>-1896252474682313</v>
+        <v>12.66666666666668</v>
       </c>
       <c r="Y70">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="71" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A71">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B71">
-        <v>1896252474682314</v>
+        <v>4.3333333333333401</v>
       </c>
       <c r="C71">
         <v>0</v>
       </c>
       <c r="D71">
-        <v>-1896252474682326</v>
+        <v>1</v>
       </c>
       <c r="E71">
         <v>0</v>
@@ -29608,13 +29576,13 @@
         <v>0</v>
       </c>
       <c r="K71">
-        <v>1</v>
+        <v>-0.50000000000000111</v>
       </c>
       <c r="L71">
-        <v>-1.368421052631581</v>
+        <v>1.000000000000004</v>
       </c>
       <c r="M71">
-        <v>0</v>
+        <v>-0.50000000000000333</v>
       </c>
       <c r="N71">
         <v>0</v>
@@ -29635,16 +29603,16 @@
         <v>0</v>
       </c>
       <c r="T71">
-        <v>13.684210526315869</v>
+        <v>-5.3333333333333401</v>
       </c>
       <c r="U71">
-        <v>-948126237341162.38</v>
+        <v>0</v>
       </c>
       <c r="V71">
-        <v>948126237341162.38</v>
+        <v>0</v>
       </c>
       <c r="W71">
-        <v>1896252474682311</v>
+        <v>5.3333333333333401</v>
       </c>
     </row>
     <row r="72" spans="1:25" x14ac:dyDescent="0.3">
@@ -29652,13 +29620,13 @@
         <v>3</v>
       </c>
       <c r="B72">
-        <v>-0.2052631578947369</v>
+        <v>-0.2</v>
       </c>
       <c r="C72">
         <v>0</v>
       </c>
       <c r="D72">
-        <v>5.2631578947368264E-3</v>
+        <v>0</v>
       </c>
       <c r="E72">
         <v>1</v>
@@ -29679,13 +29647,13 @@
         <v>0</v>
       </c>
       <c r="K72">
-        <v>0</v>
+        <v>1.7347234759768071E-18</v>
       </c>
       <c r="L72">
-        <v>5.1859101808148921E-18</v>
+        <v>1.0408340855860839E-17</v>
       </c>
       <c r="M72">
-        <v>0</v>
+        <v>-1.7347234759768071E-18</v>
       </c>
       <c r="N72">
         <v>-0.5</v>
@@ -29709,13 +29677,13 @@
         <v>-0.8</v>
       </c>
       <c r="U72">
-        <v>2.631578947368424E-3</v>
+        <v>-6.9388939039072284E-18</v>
       </c>
       <c r="V72">
-        <v>-2.631578947368424E-3</v>
+        <v>6.9388939039072284E-18</v>
       </c>
       <c r="W72">
-        <v>0.79473684210526319</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="73" spans="1:25" x14ac:dyDescent="0.3">
@@ -29723,13 +29691,13 @@
         <v>4</v>
       </c>
       <c r="B73">
-        <v>6.315789473684208E-2</v>
+        <v>1.466666666666669</v>
       </c>
       <c r="C73">
         <v>0</v>
       </c>
       <c r="D73">
-        <v>0.33684210526315822</v>
+        <v>0</v>
       </c>
       <c r="E73">
         <v>0</v>
@@ -29750,13 +29718,13 @@
         <v>0</v>
       </c>
       <c r="K73">
-        <v>0</v>
+        <v>-0.1000000000000003</v>
       </c>
       <c r="L73">
-        <v>1.54262567632127E-16</v>
+        <v>0.20000000000000129</v>
       </c>
       <c r="M73">
-        <v>0</v>
+        <v>-0.100000000000001</v>
       </c>
       <c r="N73">
         <v>0.5</v>
@@ -29777,16 +29745,16 @@
         <v>-0.5</v>
       </c>
       <c r="T73">
-        <v>-1.4</v>
+        <v>-2.466666666666669</v>
       </c>
       <c r="U73">
-        <v>0.26842105263157912</v>
+        <v>0</v>
       </c>
       <c r="V73">
-        <v>-0.26842105263157912</v>
+        <v>0</v>
       </c>
       <c r="W73">
-        <v>0.86315789473684212</v>
+        <v>2.466666666666669</v>
       </c>
     </row>
     <row r="74" spans="1:25" x14ac:dyDescent="0.3">
@@ -29794,13 +29762,13 @@
         <v>5</v>
       </c>
       <c r="B74">
-        <v>1.497340263474718E-17</v>
+        <v>0.86666666666666803</v>
       </c>
       <c r="C74">
         <v>0</v>
       </c>
       <c r="D74">
-        <v>-0.20000000000000009</v>
+        <v>0</v>
       </c>
       <c r="E74">
         <v>0</v>
@@ -29821,13 +29789,13 @@
         <v>0</v>
       </c>
       <c r="K74">
-        <v>0</v>
+        <v>-0.1000000000000002</v>
       </c>
       <c r="L74">
-        <v>-4.1633363423443383E-17</v>
+        <v>0.20000000000000079</v>
       </c>
       <c r="M74">
-        <v>0</v>
+        <v>-0.1000000000000007</v>
       </c>
       <c r="N74">
         <v>0</v>
@@ -29848,16 +29816,16 @@
         <v>0.5</v>
       </c>
       <c r="T74">
-        <v>-0.8</v>
+        <v>-1.866666666666668</v>
       </c>
       <c r="U74">
-        <v>-3.3507553457025772E-17</v>
+        <v>-2.775557561562891E-17</v>
       </c>
       <c r="V74">
-        <v>3.3507553457025772E-17</v>
+        <v>2.775557561562891E-17</v>
       </c>
       <c r="W74">
-        <v>0.80000000000000016</v>
+        <v>1.866666666666668</v>
       </c>
     </row>
     <row r="75" spans="1:25" x14ac:dyDescent="0.3">
@@ -29865,13 +29833,13 @@
         <v>6</v>
       </c>
       <c r="B75">
-        <v>-0.2052631578947369</v>
+        <v>-0.2</v>
       </c>
       <c r="C75">
         <v>0</v>
       </c>
       <c r="D75">
-        <v>5.2631578947368264E-3</v>
+        <v>0</v>
       </c>
       <c r="E75">
         <v>0</v>
@@ -29892,13 +29860,13 @@
         <v>0</v>
       </c>
       <c r="K75">
-        <v>0</v>
+        <v>1.7347234759768071E-18</v>
       </c>
       <c r="L75">
-        <v>5.1859101808148921E-18</v>
+        <v>1.0408340855860839E-17</v>
       </c>
       <c r="M75">
-        <v>0</v>
+        <v>-1.7347234759768071E-18</v>
       </c>
       <c r="N75">
         <v>0.5</v>
@@ -29922,13 +29890,13 @@
         <v>-0.8</v>
       </c>
       <c r="U75">
-        <v>2.631578947368424E-3</v>
+        <v>-6.9388939039072284E-18</v>
       </c>
       <c r="V75">
-        <v>-2.631578947368424E-3</v>
+        <v>6.9388939039072284E-18</v>
       </c>
       <c r="W75">
-        <v>0.79473684210526319</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="76" spans="1:25" x14ac:dyDescent="0.3">
@@ -29936,13 +29904,13 @@
         <v>7</v>
       </c>
       <c r="B76">
-        <v>6.315789473684208E-2</v>
+        <v>1.466666666666669</v>
       </c>
       <c r="C76">
         <v>0</v>
       </c>
       <c r="D76">
-        <v>0.33684210526315822</v>
+        <v>0</v>
       </c>
       <c r="E76">
         <v>0</v>
@@ -29963,13 +29931,13 @@
         <v>0</v>
       </c>
       <c r="K76">
-        <v>0</v>
+        <v>-0.1000000000000003</v>
       </c>
       <c r="L76">
-        <v>1.54262567632127E-16</v>
+        <v>0.20000000000000129</v>
       </c>
       <c r="M76">
-        <v>0</v>
+        <v>-0.100000000000001</v>
       </c>
       <c r="N76">
         <v>-0.5</v>
@@ -29990,16 +29958,16 @@
         <v>0.5</v>
       </c>
       <c r="T76">
-        <v>-1.4</v>
+        <v>-2.466666666666669</v>
       </c>
       <c r="U76">
-        <v>0.26842105263157912</v>
+        <v>0</v>
       </c>
       <c r="V76">
-        <v>-0.26842105263157912</v>
+        <v>0</v>
       </c>
       <c r="W76">
-        <v>0.86315789473684212</v>
+        <v>2.466666666666669</v>
       </c>
     </row>
     <row r="77" spans="1:25" x14ac:dyDescent="0.3">
@@ -30007,13 +29975,13 @@
         <v>8</v>
       </c>
       <c r="B77">
-        <v>1.497340263474718E-17</v>
+        <v>0.86666666666666803</v>
       </c>
       <c r="C77">
         <v>0</v>
       </c>
       <c r="D77">
-        <v>-0.20000000000000009</v>
+        <v>0</v>
       </c>
       <c r="E77">
         <v>0</v>
@@ -30034,13 +30002,13 @@
         <v>1</v>
       </c>
       <c r="K77">
-        <v>0</v>
+        <v>-0.1000000000000002</v>
       </c>
       <c r="L77">
-        <v>-4.1633363423443383E-17</v>
+        <v>0.20000000000000079</v>
       </c>
       <c r="M77">
-        <v>0</v>
+        <v>-0.1000000000000007</v>
       </c>
       <c r="N77">
         <v>0</v>
@@ -30061,238 +30029,729 @@
         <v>-0.5</v>
       </c>
       <c r="T77">
+        <v>-1.866666666666668</v>
+      </c>
+      <c r="U77">
+        <v>-2.775557561562891E-17</v>
+      </c>
+      <c r="V77">
+        <v>2.775557561562891E-17</v>
+      </c>
+      <c r="W77">
+        <v>1.866666666666668</v>
+      </c>
+    </row>
+    <row r="79" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B79">
+        <v>0</v>
+      </c>
+      <c r="C79">
+        <v>1</v>
+      </c>
+      <c r="D79">
+        <v>2</v>
+      </c>
+      <c r="E79">
+        <v>3</v>
+      </c>
+      <c r="F79">
+        <v>4</v>
+      </c>
+      <c r="G79">
+        <v>5</v>
+      </c>
+      <c r="H79">
+        <v>6</v>
+      </c>
+      <c r="I79">
+        <v>7</v>
+      </c>
+      <c r="J79">
+        <v>8</v>
+      </c>
+      <c r="K79">
+        <v>9</v>
+      </c>
+      <c r="L79">
+        <v>10</v>
+      </c>
+      <c r="M79">
+        <v>11</v>
+      </c>
+      <c r="N79">
+        <v>12</v>
+      </c>
+      <c r="O79">
+        <v>13</v>
+      </c>
+      <c r="P79">
+        <v>14</v>
+      </c>
+      <c r="Q79">
+        <v>15</v>
+      </c>
+      <c r="R79">
+        <v>16</v>
+      </c>
+      <c r="S79">
+        <v>17</v>
+      </c>
+      <c r="T79">
+        <v>18</v>
+      </c>
+      <c r="U79">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="80" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>1</v>
+      </c>
+      <c r="B80">
+        <v>1.9999999999999989</v>
+      </c>
+      <c r="C80">
+        <v>1</v>
+      </c>
+      <c r="D80">
+        <v>0</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+      <c r="F80">
+        <v>0</v>
+      </c>
+      <c r="G80">
+        <v>0</v>
+      </c>
+      <c r="H80">
+        <v>0</v>
+      </c>
+      <c r="I80">
+        <v>0</v>
+      </c>
+      <c r="J80">
+        <v>0</v>
+      </c>
+      <c r="K80">
+        <v>0</v>
+      </c>
+      <c r="L80">
+        <v>1.332267629550188E-15</v>
+      </c>
+      <c r="M80">
+        <v>-8.8817841970012523E-16</v>
+      </c>
+      <c r="N80">
+        <v>0</v>
+      </c>
+      <c r="O80">
+        <v>0</v>
+      </c>
+      <c r="P80">
+        <v>0</v>
+      </c>
+      <c r="Q80">
+        <v>0</v>
+      </c>
+      <c r="R80">
+        <v>0</v>
+      </c>
+      <c r="S80">
+        <v>0</v>
+      </c>
+      <c r="T80">
+        <v>-2.9999999999999991</v>
+      </c>
+      <c r="U80">
+        <v>0.50000000000000011</v>
+      </c>
+      <c r="V80">
+        <v>-0.50000000000000011</v>
+      </c>
+      <c r="W80">
+        <v>2</v>
+      </c>
+      <c r="Y80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>9</v>
+      </c>
+      <c r="B81">
+        <v>-10.66666666666665</v>
+      </c>
+      <c r="C81">
+        <v>0</v>
+      </c>
+      <c r="D81">
+        <v>0</v>
+      </c>
+      <c r="E81">
+        <v>0</v>
+      </c>
+      <c r="F81">
+        <v>0</v>
+      </c>
+      <c r="G81">
+        <v>0</v>
+      </c>
+      <c r="H81">
+        <v>0</v>
+      </c>
+      <c r="I81">
+        <v>0</v>
+      </c>
+      <c r="J81">
+        <v>0</v>
+      </c>
+      <c r="K81">
+        <v>1</v>
+      </c>
+      <c r="L81">
+        <v>-2.000000000000004</v>
+      </c>
+      <c r="M81">
+        <v>1.0000000000000051</v>
+      </c>
+      <c r="N81">
+        <v>0</v>
+      </c>
+      <c r="O81">
+        <v>0</v>
+      </c>
+      <c r="P81">
+        <v>0</v>
+      </c>
+      <c r="Q81">
+        <v>0</v>
+      </c>
+      <c r="R81">
+        <v>0</v>
+      </c>
+      <c r="S81">
+        <v>0</v>
+      </c>
+      <c r="T81">
+        <v>10.66666666666665</v>
+      </c>
+      <c r="U81">
+        <v>0.99999999999999711</v>
+      </c>
+      <c r="V81">
+        <v>-0.99999999999999711</v>
+      </c>
+      <c r="W81">
+        <v>-12.66666666666665</v>
+      </c>
+      <c r="X81">
+        <v>-12.666666666666581</v>
+      </c>
+      <c r="Y81">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="82" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>10</v>
+      </c>
+      <c r="B82">
+        <v>-0.99999999999999822</v>
+      </c>
+      <c r="C82">
+        <v>0</v>
+      </c>
+      <c r="D82">
+        <v>1</v>
+      </c>
+      <c r="E82">
+        <v>0</v>
+      </c>
+      <c r="F82">
+        <v>0</v>
+      </c>
+      <c r="G82">
+        <v>0</v>
+      </c>
+      <c r="H82">
+        <v>0</v>
+      </c>
+      <c r="I82">
+        <v>0</v>
+      </c>
+      <c r="J82">
+        <v>0</v>
+      </c>
+      <c r="K82">
+        <v>0</v>
+      </c>
+      <c r="L82">
+        <v>0</v>
+      </c>
+      <c r="M82">
+        <v>4.4408920985006262E-16</v>
+      </c>
+      <c r="N82">
+        <v>0</v>
+      </c>
+      <c r="O82">
+        <v>0</v>
+      </c>
+      <c r="P82">
+        <v>0</v>
+      </c>
+      <c r="Q82">
+        <v>0</v>
+      </c>
+      <c r="R82">
+        <v>0</v>
+      </c>
+      <c r="S82">
+        <v>0</v>
+      </c>
+      <c r="T82">
+        <v>-1.7763568394002501E-15</v>
+      </c>
+      <c r="U82">
+        <v>0.49999999999999972</v>
+      </c>
+      <c r="V82">
+        <v>-0.49999999999999972</v>
+      </c>
+      <c r="W82">
+        <v>-0.99999999999999734</v>
+      </c>
+    </row>
+    <row r="83" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>3</v>
+      </c>
+      <c r="B83">
+        <v>-0.2</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
+      <c r="E83">
+        <v>1</v>
+      </c>
+      <c r="F83">
+        <v>0</v>
+      </c>
+      <c r="G83">
+        <v>0</v>
+      </c>
+      <c r="H83">
+        <v>0</v>
+      </c>
+      <c r="I83">
+        <v>0</v>
+      </c>
+      <c r="J83">
+        <v>0</v>
+      </c>
+      <c r="K83">
+        <v>0</v>
+      </c>
+      <c r="L83">
+        <v>1.387778780781446E-17</v>
+      </c>
+      <c r="M83">
+        <v>-3.4694469519536227E-18</v>
+      </c>
+      <c r="N83">
+        <v>-0.5</v>
+      </c>
+      <c r="O83">
+        <v>0.5</v>
+      </c>
+      <c r="P83">
+        <v>0</v>
+      </c>
+      <c r="Q83">
+        <v>0.5</v>
+      </c>
+      <c r="R83">
+        <v>-0.5</v>
+      </c>
+      <c r="S83">
+        <v>0</v>
+      </c>
+      <c r="T83">
         <v>-0.8</v>
       </c>
-      <c r="U77">
-        <v>-3.3507553457025772E-17</v>
-      </c>
-      <c r="V77">
-        <v>3.3507553457025772E-17</v>
-      </c>
-      <c r="W77">
-        <v>0.80000000000000016</v>
-      </c>
-    </row>
-    <row r="80" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B80" s="3"/>
-      <c r="C80" s="3"/>
-      <c r="D80" s="3"/>
-      <c r="E80" s="3"/>
-      <c r="F80" s="3"/>
-      <c r="G80" s="3"/>
-      <c r="H80" s="3"/>
-      <c r="I80" s="3"/>
-      <c r="J80" s="3"/>
-      <c r="K80" s="3"/>
-      <c r="L80" s="3"/>
-      <c r="M80" s="3"/>
-      <c r="N80" s="3"/>
-      <c r="O80" s="3"/>
-      <c r="P80" s="3"/>
-      <c r="Q80" s="3"/>
-      <c r="R80" s="3"/>
-      <c r="S80" s="3"/>
-      <c r="T80" s="3"/>
-      <c r="U80" s="3"/>
-      <c r="V80" s="3"/>
-      <c r="W80" s="3"/>
-    </row>
-    <row r="81" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B81" s="2"/>
-      <c r="C81" s="2"/>
-      <c r="D81" s="2"/>
-      <c r="E81" s="2"/>
-      <c r="F81" s="2"/>
-      <c r="G81" s="2"/>
-      <c r="H81" s="2"/>
-      <c r="I81" s="2"/>
-      <c r="J81" s="3"/>
-      <c r="K81" s="2"/>
-      <c r="L81" s="2"/>
-      <c r="M81" s="2"/>
-      <c r="N81" s="2"/>
-      <c r="O81" s="2"/>
-      <c r="P81" s="2"/>
-      <c r="Q81" s="2"/>
-      <c r="R81" s="2"/>
-      <c r="S81" s="2"/>
-      <c r="T81" s="2"/>
-      <c r="U81" s="2"/>
-      <c r="V81" s="2"/>
-      <c r="W81" s="2"/>
-    </row>
-    <row r="82" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B82" s="2"/>
-      <c r="C82" s="2"/>
-      <c r="D82" s="2"/>
-      <c r="E82" s="2"/>
-      <c r="F82" s="2"/>
-      <c r="G82" s="2"/>
-      <c r="H82" s="2"/>
-      <c r="I82" s="2"/>
-      <c r="J82" s="3"/>
-      <c r="K82" s="2"/>
-      <c r="L82" s="2"/>
-      <c r="M82" s="2"/>
-      <c r="N82" s="2"/>
-      <c r="O82" s="2"/>
-      <c r="P82" s="2"/>
-      <c r="Q82" s="2"/>
-      <c r="R82" s="2"/>
-      <c r="S82" s="2"/>
-      <c r="T82" s="2"/>
-      <c r="U82" s="2"/>
-      <c r="V82" s="2"/>
-      <c r="W82" s="2"/>
-    </row>
-    <row r="83" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B83" s="2"/>
-      <c r="C83" s="2"/>
-      <c r="D83" s="2"/>
-      <c r="E83" s="2"/>
-      <c r="F83" s="2"/>
-      <c r="G83" s="2"/>
-      <c r="H83" s="2"/>
-      <c r="I83" s="4"/>
-      <c r="J83" s="3"/>
-      <c r="K83" s="2"/>
-      <c r="L83" s="2"/>
-      <c r="M83" s="2"/>
-      <c r="N83" s="2"/>
-      <c r="O83" s="2"/>
-      <c r="P83" s="2"/>
-      <c r="Q83" s="2"/>
-      <c r="R83" s="2"/>
-      <c r="S83" s="2"/>
-      <c r="T83" s="2"/>
-      <c r="U83" s="2"/>
-      <c r="V83" s="2"/>
-      <c r="W83" s="2"/>
-    </row>
-    <row r="84" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B84" s="2"/>
-      <c r="C84" s="2"/>
-      <c r="D84" s="2"/>
-      <c r="E84" s="2"/>
-      <c r="F84" s="2"/>
-      <c r="G84" s="2"/>
-      <c r="H84" s="2"/>
-      <c r="I84" s="2"/>
-      <c r="J84" s="3"/>
-      <c r="K84" s="2"/>
-      <c r="L84" s="2"/>
-      <c r="M84" s="2"/>
-      <c r="N84" s="2"/>
-      <c r="O84" s="2"/>
-      <c r="P84" s="2"/>
-      <c r="Q84" s="2"/>
-      <c r="R84" s="2"/>
-      <c r="S84" s="2"/>
-      <c r="T84" s="2"/>
-      <c r="U84" s="2"/>
-      <c r="V84" s="2"/>
-      <c r="W84" s="2"/>
-    </row>
-    <row r="85" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B85" s="2"/>
-      <c r="C85" s="2"/>
-      <c r="D85" s="2"/>
-      <c r="E85" s="2"/>
-      <c r="F85" s="2"/>
-      <c r="G85" s="2"/>
-      <c r="H85" s="2"/>
-      <c r="I85" s="2"/>
-      <c r="J85" s="3"/>
-      <c r="K85" s="4"/>
-      <c r="L85" s="4"/>
-      <c r="M85" s="2"/>
-      <c r="N85" s="2"/>
-      <c r="O85" s="2"/>
-      <c r="P85" s="2"/>
-      <c r="Q85" s="2"/>
-      <c r="R85" s="2"/>
-      <c r="S85" s="2"/>
-      <c r="T85" s="4"/>
-      <c r="U85" s="2"/>
-      <c r="V85" s="4"/>
-      <c r="W85" s="2"/>
-    </row>
-    <row r="86" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B86" s="2"/>
-      <c r="C86" s="2"/>
-      <c r="D86" s="2"/>
-      <c r="E86" s="2"/>
-      <c r="F86" s="2"/>
-      <c r="G86" s="2"/>
-      <c r="H86" s="2"/>
-      <c r="I86" s="2"/>
-      <c r="J86" s="3"/>
-      <c r="K86" s="2"/>
-      <c r="L86" s="2"/>
-      <c r="M86" s="2"/>
-      <c r="N86" s="2"/>
-      <c r="O86" s="2"/>
-      <c r="P86" s="2"/>
-      <c r="Q86" s="2"/>
-      <c r="R86" s="2"/>
-      <c r="S86" s="2"/>
-      <c r="T86" s="2"/>
-      <c r="U86" s="2"/>
-      <c r="V86" s="2"/>
-      <c r="W86" s="2"/>
-    </row>
-    <row r="87" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B87" s="2"/>
-      <c r="C87" s="2"/>
-      <c r="D87" s="2"/>
-      <c r="E87" s="2"/>
-      <c r="F87" s="2"/>
-      <c r="G87" s="2"/>
-      <c r="H87" s="2"/>
-      <c r="I87" s="2"/>
-      <c r="J87" s="3"/>
-      <c r="K87" s="2"/>
-      <c r="L87" s="2"/>
-      <c r="M87" s="2"/>
-      <c r="N87" s="2"/>
-      <c r="O87" s="2"/>
-      <c r="P87" s="2"/>
-      <c r="Q87" s="2"/>
-      <c r="R87" s="2"/>
-      <c r="S87" s="2"/>
-      <c r="T87" s="2"/>
-      <c r="U87" s="2"/>
-      <c r="V87" s="2"/>
-      <c r="W87" s="16"/>
-    </row>
-    <row r="88" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B88" s="2"/>
-      <c r="C88" s="2"/>
-      <c r="D88" s="2"/>
-      <c r="E88" s="2"/>
-      <c r="F88" s="2"/>
-      <c r="G88" s="2"/>
-      <c r="H88" s="2"/>
-      <c r="I88" s="4"/>
-      <c r="J88" s="3"/>
-      <c r="K88" s="4"/>
-      <c r="L88" s="4"/>
-      <c r="M88" s="4"/>
-      <c r="N88" s="4"/>
-      <c r="O88" s="2"/>
-      <c r="P88" s="2"/>
-      <c r="Q88" s="4"/>
-      <c r="R88" s="2"/>
-      <c r="S88" s="2"/>
-      <c r="T88" s="2"/>
-      <c r="U88" s="2"/>
-      <c r="V88" s="4"/>
-      <c r="W88" s="2"/>
-    </row>
-    <row r="90" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="X90" s="6"/>
-    </row>
-    <row r="91" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="U83">
+        <v>-8.6736173798840308E-18</v>
+      </c>
+      <c r="V83">
+        <v>8.6736173798840308E-18</v>
+      </c>
+      <c r="W83">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="84" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>4</v>
+      </c>
+      <c r="B84">
+        <v>0.39999999999999991</v>
+      </c>
+      <c r="C84">
+        <v>0</v>
+      </c>
+      <c r="D84">
+        <v>0</v>
+      </c>
+      <c r="E84">
+        <v>0</v>
+      </c>
+      <c r="F84">
+        <v>1</v>
+      </c>
+      <c r="G84">
+        <v>0</v>
+      </c>
+      <c r="H84">
+        <v>0</v>
+      </c>
+      <c r="I84">
+        <v>0</v>
+      </c>
+      <c r="J84">
+        <v>0</v>
+      </c>
+      <c r="K84">
+        <v>0</v>
+      </c>
+      <c r="L84">
+        <v>3.05311331771918E-16</v>
+      </c>
+      <c r="M84">
+        <v>-1.9428902930940239E-16</v>
+      </c>
+      <c r="N84">
+        <v>0.5</v>
+      </c>
+      <c r="O84">
+        <v>-1</v>
+      </c>
+      <c r="P84">
+        <v>0.5</v>
+      </c>
+      <c r="Q84">
+        <v>-0.5</v>
+      </c>
+      <c r="R84">
+        <v>1</v>
+      </c>
+      <c r="S84">
+        <v>-0.5</v>
+      </c>
+      <c r="T84">
+        <v>-1.4</v>
+      </c>
+      <c r="U84">
+        <v>0.1</v>
+      </c>
+      <c r="V84">
+        <v>-0.1</v>
+      </c>
+      <c r="W84">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>5</v>
+      </c>
+      <c r="B85">
+        <v>-0.19999999999999971</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+      <c r="E85">
+        <v>0</v>
+      </c>
+      <c r="F85">
+        <v>0</v>
+      </c>
+      <c r="G85">
+        <v>1</v>
+      </c>
+      <c r="H85">
+        <v>0</v>
+      </c>
+      <c r="I85">
+        <v>0</v>
+      </c>
+      <c r="J85">
+        <v>0</v>
+      </c>
+      <c r="K85">
+        <v>0</v>
+      </c>
+      <c r="L85">
+        <v>-2.775557561562891E-17</v>
+      </c>
+      <c r="M85">
+        <v>9.7144514654701197E-17</v>
+      </c>
+      <c r="N85">
+        <v>0</v>
+      </c>
+      <c r="O85">
+        <v>0.5</v>
+      </c>
+      <c r="P85">
+        <v>-0.5</v>
+      </c>
+      <c r="Q85">
+        <v>0</v>
+      </c>
+      <c r="R85">
+        <v>-0.5</v>
+      </c>
+      <c r="S85">
+        <v>0.5</v>
+      </c>
+      <c r="T85">
+        <v>-0.80000000000000027</v>
+      </c>
+      <c r="U85">
+        <v>9.9999999999999922E-2</v>
+      </c>
+      <c r="V85">
+        <v>-9.9999999999999922E-2</v>
+      </c>
+      <c r="W85">
+        <v>0.60000000000000009</v>
+      </c>
+    </row>
+    <row r="86" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>6</v>
+      </c>
+      <c r="B86">
+        <v>-0.2</v>
+      </c>
+      <c r="C86">
+        <v>0</v>
+      </c>
+      <c r="D86">
+        <v>0</v>
+      </c>
+      <c r="E86">
+        <v>0</v>
+      </c>
+      <c r="F86">
+        <v>0</v>
+      </c>
+      <c r="G86">
+        <v>0</v>
+      </c>
+      <c r="H86">
+        <v>1</v>
+      </c>
+      <c r="I86">
+        <v>0</v>
+      </c>
+      <c r="J86">
+        <v>0</v>
+      </c>
+      <c r="K86">
+        <v>0</v>
+      </c>
+      <c r="L86">
+        <v>1.387778780781446E-17</v>
+      </c>
+      <c r="M86">
+        <v>-3.4694469519536227E-18</v>
+      </c>
+      <c r="N86">
+        <v>0.5</v>
+      </c>
+      <c r="O86">
+        <v>-0.5</v>
+      </c>
+      <c r="P86">
+        <v>0</v>
+      </c>
+      <c r="Q86">
+        <v>-0.5</v>
+      </c>
+      <c r="R86">
+        <v>0.5</v>
+      </c>
+      <c r="S86">
+        <v>0</v>
+      </c>
+      <c r="T86">
+        <v>-0.8</v>
+      </c>
+      <c r="U86">
+        <v>-8.6736173798840308E-18</v>
+      </c>
+      <c r="V86">
+        <v>8.6736173798840308E-18</v>
+      </c>
+      <c r="W86">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>7</v>
+      </c>
+      <c r="B87">
+        <v>0.39999999999999991</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
+      </c>
+      <c r="D87">
+        <v>0</v>
+      </c>
+      <c r="E87">
+        <v>0</v>
+      </c>
+      <c r="F87">
+        <v>0</v>
+      </c>
+      <c r="G87">
+        <v>0</v>
+      </c>
+      <c r="H87">
+        <v>0</v>
+      </c>
+      <c r="I87">
+        <v>1</v>
+      </c>
+      <c r="J87">
+        <v>0</v>
+      </c>
+      <c r="K87">
+        <v>0</v>
+      </c>
+      <c r="L87">
+        <v>3.05311331771918E-16</v>
+      </c>
+      <c r="M87">
+        <v>-1.9428902930940239E-16</v>
+      </c>
+      <c r="N87">
+        <v>-0.5</v>
+      </c>
+      <c r="O87">
+        <v>1</v>
+      </c>
+      <c r="P87">
+        <v>-0.5</v>
+      </c>
+      <c r="Q87">
+        <v>0.5</v>
+      </c>
+      <c r="R87">
+        <v>-1</v>
+      </c>
+      <c r="S87">
+        <v>0.5</v>
+      </c>
+      <c r="T87">
+        <v>-1.4</v>
+      </c>
+      <c r="U87">
+        <v>0.1</v>
+      </c>
+      <c r="V87">
+        <v>-0.1</v>
+      </c>
+      <c r="W87">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>8</v>
+      </c>
+      <c r="B88">
+        <v>-0.19999999999999971</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
+      </c>
+      <c r="E88">
+        <v>0</v>
+      </c>
+      <c r="F88">
+        <v>0</v>
+      </c>
+      <c r="G88">
+        <v>0</v>
+      </c>
+      <c r="H88">
+        <v>0</v>
+      </c>
+      <c r="I88">
+        <v>0</v>
+      </c>
+      <c r="J88">
+        <v>1</v>
+      </c>
+      <c r="K88">
+        <v>0</v>
+      </c>
+      <c r="L88">
+        <v>-2.775557561562891E-17</v>
+      </c>
+      <c r="M88">
+        <v>9.7144514654701197E-17</v>
+      </c>
+      <c r="N88">
+        <v>0</v>
+      </c>
+      <c r="O88">
+        <v>-0.5</v>
+      </c>
+      <c r="P88">
+        <v>0.5</v>
+      </c>
+      <c r="Q88">
+        <v>0</v>
+      </c>
+      <c r="R88">
+        <v>0.5</v>
+      </c>
+      <c r="S88">
+        <v>-0.5</v>
+      </c>
+      <c r="T88">
+        <v>-0.80000000000000027</v>
+      </c>
+      <c r="U88">
+        <v>9.9999999999999922E-2</v>
+      </c>
+      <c r="V88">
+        <v>-9.9999999999999922E-2</v>
+      </c>
+      <c r="W88">
+        <v>0.60000000000000009</v>
+      </c>
+    </row>
+    <row r="91" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
       <c r="D91" s="2"/>
@@ -30316,7 +30775,7 @@
       <c r="V91" s="2"/>
       <c r="W91" s="2"/>
     </row>
-    <row r="92" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
       <c r="D92" s="2"/>
@@ -30340,7 +30799,7 @@
       <c r="V92" s="4"/>
       <c r="W92" s="2"/>
     </row>
-    <row r="93" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
       <c r="D93" s="2"/>
@@ -30364,7 +30823,7 @@
       <c r="V93" s="4"/>
       <c r="W93" s="2"/>
     </row>
-    <row r="94" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
@@ -30388,7 +30847,7 @@
       <c r="V94" s="4"/>
       <c r="W94" s="4"/>
     </row>
-    <row r="95" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
       <c r="D95" s="2"/>
@@ -30412,7 +30871,7 @@
       <c r="V95" s="4"/>
       <c r="W95" s="2"/>
     </row>
-    <row r="96" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
       <c r="D96" s="2"/>

</xml_diff>

<commit_message>
Testing force inc alg v4
</commit_message>
<xml_diff>
--- a/Examples/Problems solutions.xlsx
+++ b/Examples/Problems solutions.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="71">
   <si>
     <t>xn1</t>
   </si>
@@ -175,9 +175,6 @@
     <t>как получить что p должно быть равно нулю здесь</t>
   </si>
   <si>
-    <t>pRv</t>
-  </si>
-  <si>
     <t>basis</t>
   </si>
   <si>
@@ -193,14 +190,498 @@
     <t>n</t>
   </si>
   <si>
-    <t>error, %</t>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>n1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>n2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>n3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>z</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>n1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>z</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>n2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>z</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>n3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>τ1</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>τ2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>τ3</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>τ1</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>-</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>τ2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>-</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>τ3</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>-</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>z</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>τ1</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>z</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>τ2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>z</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>τ3</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>z</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>τ1</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>-</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>z</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>τ2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>-</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>z</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>τ3</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>-</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pR</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>v</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>c</t>
+    </r>
+  </si>
+  <si>
+    <t>u error, %</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,6 +714,24 @@
     </font>
     <font>
       <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="subscript"/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="superscript"/>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -293,7 +792,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -314,6 +813,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -32961,8 +33463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="R38" sqref="R38"/>
+    <sheetView tabSelected="1" topLeftCell="O31" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="X37" sqref="X37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -32973,81 +33475,86 @@
     <col min="21" max="21" width="6.5703125" style="11" customWidth="1"/>
     <col min="22" max="22" width="8.140625" style="11" customWidth="1"/>
     <col min="23" max="24" width="9.140625" style="11"/>
-    <col min="25" max="25" width="7.42578125" style="11" customWidth="1"/>
-    <col min="26" max="16384" width="9.140625" style="11"/>
+    <col min="25" max="25" width="8.7109375" style="11" customWidth="1"/>
+    <col min="26" max="26" width="10.7109375" style="11" customWidth="1"/>
+    <col min="27" max="27" width="10.5703125" style="11" customWidth="1"/>
+    <col min="28" max="28" width="9.7109375" style="11" customWidth="1"/>
+    <col min="29" max="30" width="10.28515625" style="11" customWidth="1"/>
+    <col min="31" max="31" width="10.42578125" style="11" customWidth="1"/>
+    <col min="32" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C1" s="11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="P2" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q2" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="R2" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="S2" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="T2" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="U2" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="V2" s="12" t="s">
         <v>46</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="M2" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="N2" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="O2" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="P2" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q2" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="R2" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="S2" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="T2" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="U2" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="V2" s="12" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
@@ -33653,69 +34160,69 @@
     <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" s="14"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>5</v>
+        <v>58</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
       <c r="J13" s="12" t="s">
-        <v>8</v>
+        <v>61</v>
       </c>
       <c r="K13" s="12" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="L13" s="12" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="M13" s="12" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="N13" s="12" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="O13" s="12" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="P13" s="12" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="Q13" s="12" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="R13" s="12" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="S13" s="12" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="T13" s="12" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="U13" s="12" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
       <c r="V13" s="12" t="s">
         <v>19</v>
@@ -33848,7 +34355,7 @@
         <v>0</v>
       </c>
       <c r="T15" s="13">
-        <v>1.110223024625157E-16</v>
+        <v>0</v>
       </c>
       <c r="U15" s="13">
         <v>8.3333333333333357</v>
@@ -33916,7 +34423,7 @@
         <v>0</v>
       </c>
       <c r="T16" s="13">
-        <v>-5.5511151231257827E-17</v>
+        <v>0</v>
       </c>
       <c r="U16" s="13">
         <v>5.3333333333333348</v>
@@ -34315,69 +34822,69 @@
     <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23" s="14"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>5</v>
+        <v>58</v>
       </c>
       <c r="H24" s="12" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="I24" s="12" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
       <c r="J24" s="12" t="s">
-        <v>8</v>
+        <v>61</v>
       </c>
       <c r="K24" s="12" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="L24" s="12" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="M24" s="12" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="N24" s="12" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="O24" s="12" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="P24" s="12" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="Q24" s="12" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="R24" s="12" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="S24" s="12" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="T24" s="12" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="U24" s="12" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
       <c r="V24" s="12" t="s">
         <v>19</v>
@@ -34976,42 +35483,54 @@
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.2">
       <c r="Z36" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:31" x14ac:dyDescent="0.2">
       <c r="Y39" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z39" s="13">
+        <v>49</v>
+      </c>
+      <c r="Z39" s="16">
+        <v>5</v>
+      </c>
+      <c r="AA39" s="16">
         <v>10</v>
       </c>
-      <c r="AA39" s="13">
+      <c r="AB39" s="16">
         <v>20</v>
       </c>
-      <c r="AB39" s="13">
+      <c r="AC39" s="16">
         <v>40</v>
       </c>
-      <c r="AC39" s="13">
+      <c r="AD39" s="16">
         <v>80</v>
       </c>
-      <c r="AD39" s="13">
+      <c r="AE39" s="16">
         <v>160</v>
-      </c>
-      <c r="AE39" s="13">
-        <v>320</v>
       </c>
     </row>
     <row r="40" spans="1:31" x14ac:dyDescent="0.2">
       <c r="Y40" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z40" s="13"/>
-      <c r="AA40" s="13"/>
-      <c r="AB40" s="13"/>
-      <c r="AC40" s="13"/>
-      <c r="AD40" s="13"/>
-      <c r="AE40" s="13"/>
+        <v>70</v>
+      </c>
+      <c r="Z40" s="16">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="AA40" s="16">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="AB40" s="16">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="AC40" s="16">
+        <v>0.91</v>
+      </c>
+      <c r="AD40" s="16">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="AE40" s="16">
+        <v>0.84</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>